<commit_message>
Se añadio para editar movimiento
</commit_message>
<xml_diff>
--- a/FinancieroG.xlsx
+++ b/FinancieroG.xlsx
@@ -1,40 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Proveedores" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Resumen" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="ProveedoresCliente" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="ResumenCliente" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Gastos" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Proveedores" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resumen" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProveedoresCliente" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ResumenCliente" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Gastos" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ProveedoresCliente'!$A$1:$H$87</definedName>
+  </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -58,17 +56,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,9 +466,9 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col width="20.125" customWidth="1" style="6" min="2" max="2"/>
+    <col width="20.109375" customWidth="1" style="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -483,7 +477,7 @@
           <t>Id</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Fecha</t>
         </is>
@@ -523,7 +517,7 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="n">
+      <c r="B2" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -559,7 +553,7 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -595,7 +589,7 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="2" t="n">
         <v>45818</v>
       </c>
       <c r="C4" t="inlineStr">
@@ -631,7 +625,7 @@
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="B5" s="2" t="n">
         <v>45820</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -667,7 +661,7 @@
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="2" t="n">
         <v>45828</v>
       </c>
       <c r="C6" t="inlineStr">
@@ -703,7 +697,7 @@
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="n">
+      <c r="B7" s="2" t="n">
         <v>45843</v>
       </c>
       <c r="C7" t="inlineStr">
@@ -739,7 +733,7 @@
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="n">
+      <c r="B8" s="2" t="n">
         <v>45848</v>
       </c>
       <c r="C8" t="inlineStr">
@@ -775,7 +769,7 @@
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="2" t="n">
         <v>45849</v>
       </c>
       <c r="C9" t="inlineStr">
@@ -811,7 +805,7 @@
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="n">
+      <c r="B10" s="2" t="n">
         <v>45863</v>
       </c>
       <c r="C10" t="inlineStr">
@@ -847,7 +841,7 @@
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="n">
+      <c r="B11" s="2" t="n">
         <v>45807</v>
       </c>
       <c r="C11" t="inlineStr">
@@ -883,7 +877,7 @@
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="2" t="n">
         <v>45807</v>
       </c>
       <c r="C12" t="inlineStr">
@@ -919,7 +913,7 @@
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="2" t="n">
         <v>45722</v>
       </c>
       <c r="C13" t="inlineStr">
@@ -955,7 +949,7 @@
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="n">
+      <c r="B14" s="2" t="n">
         <v>45819</v>
       </c>
       <c r="C14" t="inlineStr">
@@ -991,7 +985,7 @@
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="n">
+      <c r="B15" s="2" t="n">
         <v>45820</v>
       </c>
       <c r="C15" t="inlineStr">
@@ -1027,7 +1021,7 @@
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="n">
+      <c r="B16" s="2" t="n">
         <v>45822</v>
       </c>
       <c r="C16" t="inlineStr">
@@ -1063,7 +1057,7 @@
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="n">
+      <c r="B17" s="2" t="n">
         <v>45822</v>
       </c>
       <c r="C17" t="inlineStr">
@@ -1099,7 +1093,7 @@
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="n">
+      <c r="B18" s="2" t="n">
         <v>45822</v>
       </c>
       <c r="C18" t="inlineStr">
@@ -1135,7 +1129,7 @@
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="n">
+      <c r="B19" s="2" t="n">
         <v>45829</v>
       </c>
       <c r="C19" t="inlineStr">
@@ -1171,7 +1165,7 @@
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="n">
+      <c r="B20" s="2" t="n">
         <v>45833</v>
       </c>
       <c r="C20" t="inlineStr">
@@ -1207,7 +1201,7 @@
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="n">
+      <c r="B21" s="2" t="n">
         <v>45836</v>
       </c>
       <c r="C21" t="inlineStr">
@@ -1243,7 +1237,7 @@
       <c r="A22" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="n">
+      <c r="B22" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C22" t="inlineStr">
@@ -1279,7 +1273,7 @@
       <c r="A23" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="n">
+      <c r="B23" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C23" t="inlineStr">
@@ -1315,7 +1309,7 @@
       <c r="A24" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="n">
+      <c r="B24" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C24" t="inlineStr">
@@ -1351,7 +1345,7 @@
       <c r="A25" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="n">
+      <c r="B25" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C25" t="inlineStr">
@@ -1387,7 +1381,7 @@
       <c r="A26" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="n">
+      <c r="B26" s="2" t="n">
         <v>45840</v>
       </c>
       <c r="C26" t="inlineStr">
@@ -1423,7 +1417,7 @@
       <c r="A27" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="n">
+      <c r="B27" s="2" t="n">
         <v>45840</v>
       </c>
       <c r="C27" t="inlineStr">
@@ -1459,7 +1453,7 @@
       <c r="A28" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="n">
+      <c r="B28" s="2" t="n">
         <v>45840</v>
       </c>
       <c r="C28" t="inlineStr">
@@ -1495,7 +1489,7 @@
       <c r="A29" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="n">
+      <c r="B29" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C29" t="inlineStr">
@@ -1531,7 +1525,7 @@
       <c r="A30" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="n">
+      <c r="B30" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C30" t="inlineStr">
@@ -1567,7 +1561,7 @@
       <c r="A31" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="n">
+      <c r="B31" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C31" t="inlineStr">
@@ -1603,7 +1597,7 @@
       <c r="A32" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="n">
+      <c r="B32" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C32" t="inlineStr">
@@ -1639,7 +1633,7 @@
       <c r="A33" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="n">
+      <c r="B33" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C33" t="inlineStr">
@@ -1675,7 +1669,7 @@
       <c r="A34" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="n">
+      <c r="B34" s="2" t="n">
         <v>45842</v>
       </c>
       <c r="C34" t="inlineStr">
@@ -1711,7 +1705,7 @@
       <c r="A35" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="n">
+      <c r="B35" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C35" t="inlineStr">
@@ -1747,7 +1741,7 @@
       <c r="A36" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="n">
+      <c r="B36" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C36" t="inlineStr">
@@ -1783,7 +1777,7 @@
       <c r="A37" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="8" t="n">
+      <c r="B37" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C37" t="inlineStr">
@@ -1819,7 +1813,7 @@
       <c r="A38" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="n">
+      <c r="B38" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C38" t="inlineStr">
@@ -1855,7 +1849,7 @@
       <c r="A39" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="n">
+      <c r="B39" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C39" t="inlineStr">
@@ -1891,7 +1885,7 @@
       <c r="A40" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="8" t="n">
+      <c r="B40" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C40" t="inlineStr">
@@ -1927,7 +1921,7 @@
       <c r="A41" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="8" t="n">
+      <c r="B41" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C41" t="inlineStr">
@@ -1963,7 +1957,7 @@
       <c r="A42" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="8" t="n">
+      <c r="B42" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C42" t="inlineStr">
@@ -1999,7 +1993,7 @@
       <c r="A43" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="8" t="n">
+      <c r="B43" s="2" t="n">
         <v>45850</v>
       </c>
       <c r="C43" t="inlineStr">
@@ -2035,7 +2029,7 @@
       <c r="A44" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="8" t="n">
+      <c r="B44" s="2" t="n">
         <v>45851</v>
       </c>
       <c r="C44" t="inlineStr">
@@ -2071,7 +2065,7 @@
       <c r="A45" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="8" t="n">
+      <c r="B45" s="2" t="n">
         <v>45861</v>
       </c>
       <c r="C45" t="inlineStr">
@@ -2107,7 +2101,7 @@
       <c r="A46" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="8" t="n">
+      <c r="B46" s="2" t="n">
         <v>45861</v>
       </c>
       <c r="C46" t="inlineStr">
@@ -2143,7 +2137,7 @@
       <c r="A47" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="8" t="n">
+      <c r="B47" s="2" t="n">
         <v>45861</v>
       </c>
       <c r="C47" t="inlineStr">
@@ -2179,7 +2173,7 @@
       <c r="A48" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="8" t="n">
+      <c r="B48" s="2" t="n">
         <v>45861</v>
       </c>
       <c r="C48" t="inlineStr">
@@ -2215,7 +2209,7 @@
       <c r="A49" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="8" t="n">
+      <c r="B49" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C49" t="inlineStr">
@@ -2251,7 +2245,7 @@
       <c r="A50" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="8" t="n">
+      <c r="B50" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C50" t="inlineStr">
@@ -2287,7 +2281,7 @@
       <c r="A51" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="8" t="n">
+      <c r="B51" s="2" t="n">
         <v>45873</v>
       </c>
       <c r="C51" t="inlineStr">
@@ -2323,7 +2317,7 @@
       <c r="A52" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="8" t="n">
+      <c r="B52" s="2" t="n">
         <v>45862</v>
       </c>
       <c r="C52" t="inlineStr">
@@ -2359,7 +2353,7 @@
       <c r="A53" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="8" t="n">
+      <c r="B53" s="2" t="n">
         <v>45864</v>
       </c>
       <c r="C53" t="inlineStr">
@@ -2395,7 +2389,7 @@
       <c r="A54" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="8" t="n">
+      <c r="B54" s="2" t="n">
         <v>45865</v>
       </c>
       <c r="C54" t="inlineStr">
@@ -2431,7 +2425,7 @@
       <c r="A55" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="8" t="n">
+      <c r="B55" s="2" t="n">
         <v>45863</v>
       </c>
       <c r="C55" t="inlineStr">
@@ -2467,7 +2461,7 @@
       <c r="A56" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="8" t="n">
+      <c r="B56" s="2" t="n">
         <v>45866</v>
       </c>
       <c r="C56" t="inlineStr">
@@ -2503,7 +2497,7 @@
       <c r="A57" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="8" t="n">
+      <c r="B57" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C57" t="inlineStr">
@@ -2539,7 +2533,7 @@
       <c r="A58" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="8" t="n">
+      <c r="B58" s="2" t="n">
         <v>45871</v>
       </c>
       <c r="C58" t="inlineStr">
@@ -2575,7 +2569,7 @@
       <c r="A59" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="8" t="n">
+      <c r="B59" s="2" t="n">
         <v>45871</v>
       </c>
       <c r="C59" t="inlineStr">
@@ -2611,7 +2605,7 @@
       <c r="A60" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="8" t="n">
+      <c r="B60" s="2" t="n">
         <v>45872</v>
       </c>
       <c r="C60" t="inlineStr">
@@ -2647,7 +2641,7 @@
       <c r="A61" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="8" t="n">
+      <c r="B61" s="2" t="n">
         <v>45828</v>
       </c>
       <c r="C61" t="inlineStr">
@@ -2683,7 +2677,7 @@
       <c r="A62" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="8" t="n">
+      <c r="B62" s="2" t="n">
         <v>45828</v>
       </c>
       <c r="C62" t="inlineStr">
@@ -2719,7 +2713,7 @@
       <c r="A63" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="8" t="n">
+      <c r="B63" s="2" t="n">
         <v>45832</v>
       </c>
       <c r="C63" t="inlineStr">
@@ -2755,7 +2749,7 @@
       <c r="A64" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="8" t="n">
+      <c r="B64" s="2" t="n">
         <v>45832</v>
       </c>
       <c r="C64" t="inlineStr">
@@ -2791,7 +2785,7 @@
       <c r="A65" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="8" t="n">
+      <c r="B65" s="2" t="n">
         <v>45820</v>
       </c>
       <c r="C65" t="inlineStr">
@@ -2827,7 +2821,7 @@
       <c r="A66" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="8" t="n">
+      <c r="B66" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C66" t="inlineStr">
@@ -2863,7 +2857,7 @@
       <c r="A67" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="8" t="n">
+      <c r="B67" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C67" t="inlineStr">
@@ -2899,7 +2893,7 @@
       <c r="A68" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="8" t="n">
+      <c r="B68" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C68" t="inlineStr">
@@ -2935,7 +2929,7 @@
       <c r="A69" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="8" t="n">
+      <c r="B69" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C69" t="inlineStr">
@@ -2971,7 +2965,7 @@
       <c r="A70" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="8" t="n">
+      <c r="B70" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C70" t="inlineStr">
@@ -3007,7 +3001,7 @@
       <c r="A71" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="8" t="n">
+      <c r="B71" s="2" t="n">
         <v>45827</v>
       </c>
       <c r="C71" t="inlineStr">
@@ -3043,7 +3037,7 @@
       <c r="A72" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="8" t="n">
+      <c r="B72" s="2" t="n">
         <v>45832</v>
       </c>
       <c r="C72" t="inlineStr">
@@ -3079,7 +3073,7 @@
       <c r="A73" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="8" t="n">
+      <c r="B73" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C73" t="inlineStr">
@@ -3115,7 +3109,7 @@
       <c r="A74" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="8" t="n">
+      <c r="B74" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C74" t="inlineStr">
@@ -3151,7 +3145,7 @@
       <c r="A75" t="n">
         <v>74</v>
       </c>
-      <c r="B75" s="8" t="n">
+      <c r="B75" s="2" t="n">
         <v>45848</v>
       </c>
       <c r="C75" t="inlineStr">
@@ -3187,7 +3181,7 @@
       <c r="A76" t="n">
         <v>75</v>
       </c>
-      <c r="B76" s="8" t="n">
+      <c r="B76" s="2" t="n">
         <v>45849</v>
       </c>
       <c r="C76" t="inlineStr">
@@ -3223,7 +3217,7 @@
       <c r="A77" t="n">
         <v>76</v>
       </c>
-      <c r="B77" s="8" t="n">
+      <c r="B77" s="2" t="n">
         <v>45860</v>
       </c>
       <c r="C77" t="inlineStr">
@@ -3259,7 +3253,7 @@
       <c r="A78" t="n">
         <v>77</v>
       </c>
-      <c r="B78" s="8" t="n">
+      <c r="B78" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C78" t="inlineStr">
@@ -3295,7 +3289,7 @@
       <c r="A79" t="n">
         <v>78</v>
       </c>
-      <c r="B79" s="8" t="n">
+      <c r="B79" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C79" t="inlineStr">
@@ -3331,7 +3325,7 @@
       <c r="A80" t="n">
         <v>79</v>
       </c>
-      <c r="B80" s="8" t="n">
+      <c r="B80" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C80" t="inlineStr">
@@ -3367,7 +3361,7 @@
       <c r="A81" t="n">
         <v>80</v>
       </c>
-      <c r="B81" s="8" t="n">
+      <c r="B81" s="2" t="n">
         <v>45868</v>
       </c>
       <c r="C81" t="inlineStr">
@@ -3403,7 +3397,7 @@
       <c r="A82" t="n">
         <v>81</v>
       </c>
-      <c r="B82" s="8" t="n">
+      <c r="B82" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C82" t="inlineStr">
@@ -3439,7 +3433,7 @@
       <c r="A83" t="n">
         <v>82</v>
       </c>
-      <c r="B83" s="8" t="n">
+      <c r="B83" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="C83" t="inlineStr">
@@ -3475,7 +3469,7 @@
       <c r="A84" t="n">
         <v>83</v>
       </c>
-      <c r="B84" s="8" t="n">
+      <c r="B84" s="2" t="n">
         <v>45828</v>
       </c>
       <c r="C84" t="inlineStr">
@@ -3511,7 +3505,7 @@
       <c r="A85" t="n">
         <v>84</v>
       </c>
-      <c r="B85" s="8" t="n">
+      <c r="B85" s="2" t="n">
         <v>45832</v>
       </c>
       <c r="C85" t="inlineStr">
@@ -3547,7 +3541,7 @@
       <c r="A86" t="n">
         <v>85</v>
       </c>
-      <c r="B86" s="8" t="n">
+      <c r="B86" s="2" t="n">
         <v>45834</v>
       </c>
       <c r="C86" t="inlineStr">
@@ -3583,7 +3577,7 @@
       <c r="A87" t="n">
         <v>86</v>
       </c>
-      <c r="B87" s="8" t="n">
+      <c r="B87" s="2" t="n">
         <v>45834</v>
       </c>
       <c r="C87" t="inlineStr">
@@ -3619,7 +3613,7 @@
       <c r="A88" t="n">
         <v>87</v>
       </c>
-      <c r="B88" s="8" t="n">
+      <c r="B88" s="2" t="n">
         <v>45834</v>
       </c>
       <c r="C88" t="inlineStr">
@@ -3655,7 +3649,7 @@
       <c r="A89" t="n">
         <v>88</v>
       </c>
-      <c r="B89" s="8" t="n">
+      <c r="B89" s="2" t="n">
         <v>45835</v>
       </c>
       <c r="C89" t="inlineStr">
@@ -3691,7 +3685,7 @@
       <c r="A90" t="n">
         <v>89</v>
       </c>
-      <c r="B90" s="8" t="n">
+      <c r="B90" s="2" t="n">
         <v>45835</v>
       </c>
       <c r="C90" t="inlineStr">
@@ -3727,7 +3721,7 @@
       <c r="A91" t="n">
         <v>90</v>
       </c>
-      <c r="B91" s="8" t="n">
+      <c r="B91" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C91" t="inlineStr">
@@ -3763,7 +3757,7 @@
       <c r="A92" t="n">
         <v>91</v>
       </c>
-      <c r="B92" s="8" t="n">
+      <c r="B92" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C92" t="inlineStr">
@@ -3799,7 +3793,7 @@
       <c r="A93" t="n">
         <v>92</v>
       </c>
-      <c r="B93" s="8" t="n">
+      <c r="B93" s="2" t="n">
         <v>45843</v>
       </c>
       <c r="C93" t="inlineStr">
@@ -3835,7 +3829,7 @@
       <c r="A94" t="n">
         <v>93</v>
       </c>
-      <c r="B94" s="8" t="n">
+      <c r="B94" s="2" t="n">
         <v>45848</v>
       </c>
       <c r="C94" t="inlineStr">
@@ -3871,7 +3865,7 @@
       <c r="A95" t="n">
         <v>94</v>
       </c>
-      <c r="B95" s="8" t="n">
+      <c r="B95" s="2" t="n">
         <v>45848</v>
       </c>
       <c r="C95" t="inlineStr">
@@ -3907,7 +3901,7 @@
       <c r="A96" t="n">
         <v>95</v>
       </c>
-      <c r="B96" s="8" t="n">
+      <c r="B96" s="2" t="n">
         <v>45861</v>
       </c>
       <c r="C96" t="inlineStr">
@@ -3943,7 +3937,7 @@
       <c r="A97" t="n">
         <v>96</v>
       </c>
-      <c r="B97" s="8" t="n">
+      <c r="B97" s="2" t="n">
         <v>45863</v>
       </c>
       <c r="C97" t="inlineStr">
@@ -3979,7 +3973,7 @@
       <c r="A98" t="n">
         <v>97</v>
       </c>
-      <c r="B98" s="8" t="n">
+      <c r="B98" s="2" t="n">
         <v>45815</v>
       </c>
       <c r="C98" t="inlineStr">
@@ -4015,7 +4009,7 @@
       <c r="A99" t="n">
         <v>98</v>
       </c>
-      <c r="B99" s="8" t="n">
+      <c r="B99" s="2" t="n">
         <v>45813</v>
       </c>
       <c r="C99" t="inlineStr">
@@ -4051,7 +4045,7 @@
       <c r="A100" t="n">
         <v>99</v>
       </c>
-      <c r="B100" s="8" t="n">
+      <c r="B100" s="2" t="n">
         <v>45814</v>
       </c>
       <c r="C100" t="inlineStr">
@@ -4087,7 +4081,7 @@
       <c r="A101" t="n">
         <v>100</v>
       </c>
-      <c r="B101" s="8" t="n">
+      <c r="B101" s="2" t="n">
         <v>45814</v>
       </c>
       <c r="C101" t="inlineStr">
@@ -4123,7 +4117,7 @@
       <c r="A102" t="n">
         <v>101</v>
       </c>
-      <c r="B102" s="8" t="n">
+      <c r="B102" s="2" t="n">
         <v>45815</v>
       </c>
       <c r="C102" t="inlineStr">
@@ -4159,7 +4153,7 @@
       <c r="A103" t="n">
         <v>102</v>
       </c>
-      <c r="B103" s="8" t="n">
+      <c r="B103" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C103" t="inlineStr">
@@ -4195,7 +4189,7 @@
       <c r="A104" t="n">
         <v>103</v>
       </c>
-      <c r="B104" s="8" t="n">
+      <c r="B104" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C104" t="inlineStr">
@@ -4231,7 +4225,7 @@
       <c r="A105" t="n">
         <v>104</v>
       </c>
-      <c r="B105" s="8" t="n">
+      <c r="B105" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C105" t="inlineStr">
@@ -4267,7 +4261,7 @@
       <c r="A106" t="n">
         <v>105</v>
       </c>
-      <c r="B106" s="8" t="n">
+      <c r="B106" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C106" t="inlineStr">
@@ -4303,7 +4297,7 @@
       <c r="A107" t="n">
         <v>106</v>
       </c>
-      <c r="B107" s="8" t="n">
+      <c r="B107" s="2" t="n">
         <v>45819</v>
       </c>
       <c r="C107" t="inlineStr">
@@ -4339,7 +4333,7 @@
       <c r="A108" t="n">
         <v>107</v>
       </c>
-      <c r="B108" s="8" t="n">
+      <c r="B108" s="2" t="n">
         <v>45821</v>
       </c>
       <c r="C108" t="inlineStr">
@@ -4375,7 +4369,7 @@
       <c r="A109" t="n">
         <v>108</v>
       </c>
-      <c r="B109" s="8" t="n">
+      <c r="B109" s="2" t="n">
         <v>45822</v>
       </c>
       <c r="C109" t="inlineStr">
@@ -4411,7 +4405,7 @@
       <c r="A110" t="n">
         <v>109</v>
       </c>
-      <c r="B110" s="8" t="n">
+      <c r="B110" s="2" t="n">
         <v>45822</v>
       </c>
       <c r="C110" t="inlineStr">
@@ -4447,7 +4441,7 @@
       <c r="A111" t="n">
         <v>110</v>
       </c>
-      <c r="B111" s="8" t="n">
+      <c r="B111" s="2" t="n">
         <v>45826</v>
       </c>
       <c r="C111" t="inlineStr">
@@ -4483,7 +4477,7 @@
       <c r="A112" t="n">
         <v>111</v>
       </c>
-      <c r="B112" s="8" t="n">
+      <c r="B112" s="2" t="n">
         <v>45835</v>
       </c>
       <c r="C112" t="inlineStr">
@@ -4519,7 +4513,7 @@
       <c r="A113" t="n">
         <v>112</v>
       </c>
-      <c r="B113" s="8" t="n">
+      <c r="B113" s="2" t="n">
         <v>45835</v>
       </c>
       <c r="C113" t="inlineStr">
@@ -4555,7 +4549,7 @@
       <c r="A114" t="n">
         <v>113</v>
       </c>
-      <c r="B114" s="8" t="n">
+      <c r="B114" s="2" t="n">
         <v>45848</v>
       </c>
       <c r="C114" t="inlineStr">
@@ -4591,7 +4585,7 @@
       <c r="A115" t="n">
         <v>114</v>
       </c>
-      <c r="B115" s="8" t="n">
+      <c r="B115" s="2" t="n">
         <v>45842</v>
       </c>
       <c r="C115" t="inlineStr">
@@ -4627,7 +4621,7 @@
       <c r="A116" t="n">
         <v>115</v>
       </c>
-      <c r="B116" s="8" t="n">
+      <c r="B116" s="2" t="n">
         <v>45842</v>
       </c>
       <c r="C116" t="inlineStr">
@@ -4663,7 +4657,7 @@
       <c r="A117" t="n">
         <v>116</v>
       </c>
-      <c r="B117" s="8" t="n">
+      <c r="B117" s="2" t="n">
         <v>45842</v>
       </c>
       <c r="C117" t="inlineStr">
@@ -4699,7 +4693,7 @@
       <c r="A118" t="n">
         <v>117</v>
       </c>
-      <c r="B118" s="8" t="n">
+      <c r="B118" s="2" t="n">
         <v>45843</v>
       </c>
       <c r="C118" t="inlineStr">
@@ -4735,7 +4729,7 @@
       <c r="A119" t="n">
         <v>118</v>
       </c>
-      <c r="B119" s="8" t="n">
+      <c r="B119" s="2" t="n">
         <v>45843</v>
       </c>
       <c r="C119" t="inlineStr">
@@ -4771,7 +4765,7 @@
       <c r="A120" t="n">
         <v>119</v>
       </c>
-      <c r="B120" s="8" t="n">
+      <c r="B120" s="2" t="n">
         <v>45846</v>
       </c>
       <c r="C120" t="inlineStr">
@@ -4807,7 +4801,7 @@
       <c r="A121" t="n">
         <v>120</v>
       </c>
-      <c r="B121" s="8" t="n">
+      <c r="B121" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C121" t="inlineStr">
@@ -4843,7 +4837,7 @@
       <c r="A122" t="n">
         <v>121</v>
       </c>
-      <c r="B122" s="8" t="n">
+      <c r="B122" s="2" t="n">
         <v>45849</v>
       </c>
       <c r="C122" t="inlineStr">
@@ -4879,7 +4873,7 @@
       <c r="A123" t="n">
         <v>122</v>
       </c>
-      <c r="B123" s="8" t="n">
+      <c r="B123" s="2" t="n">
         <v>45849</v>
       </c>
       <c r="C123" t="inlineStr">
@@ -4915,7 +4909,7 @@
       <c r="A124" t="n">
         <v>123</v>
       </c>
-      <c r="B124" s="8" t="n">
+      <c r="B124" s="2" t="n">
         <v>45850</v>
       </c>
       <c r="C124" t="inlineStr">
@@ -4951,7 +4945,7 @@
       <c r="A125" t="n">
         <v>124</v>
       </c>
-      <c r="B125" s="8" t="n">
+      <c r="B125" s="2" t="n">
         <v>45863</v>
       </c>
       <c r="C125" t="inlineStr">
@@ -4987,7 +4981,7 @@
       <c r="A126" t="n">
         <v>125</v>
       </c>
-      <c r="B126" s="8" t="n">
+      <c r="B126" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C126" t="inlineStr">
@@ -5023,7 +5017,7 @@
       <c r="A127" t="n">
         <v>126</v>
       </c>
-      <c r="B127" s="8" t="n">
+      <c r="B127" s="2" t="n">
         <v>45863</v>
       </c>
       <c r="C127" t="inlineStr">
@@ -5059,7 +5053,7 @@
       <c r="A128" t="n">
         <v>127</v>
       </c>
-      <c r="B128" s="8" t="n">
+      <c r="B128" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C128" t="inlineStr">
@@ -5095,7 +5089,7 @@
       <c r="A129" t="n">
         <v>128</v>
       </c>
-      <c r="B129" s="8" t="n">
+      <c r="B129" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C129" t="inlineStr">
@@ -5131,7 +5125,7 @@
       <c r="A130" t="n">
         <v>129</v>
       </c>
-      <c r="B130" s="8" t="n">
+      <c r="B130" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C130" t="inlineStr">
@@ -5167,7 +5161,7 @@
       <c r="A131" t="n">
         <v>130</v>
       </c>
-      <c r="B131" s="8" t="n">
+      <c r="B131" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C131" t="inlineStr">
@@ -5203,7 +5197,7 @@
       <c r="A132" t="n">
         <v>131</v>
       </c>
-      <c r="B132" s="8" t="n">
+      <c r="B132" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C132" t="inlineStr">
@@ -5239,7 +5233,7 @@
       <c r="A133" t="n">
         <v>132</v>
       </c>
-      <c r="B133" s="8" t="n">
+      <c r="B133" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C133" t="inlineStr">
@@ -5275,7 +5269,7 @@
       <c r="A134" t="n">
         <v>133</v>
       </c>
-      <c r="B134" s="8" t="n">
+      <c r="B134" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C134" t="inlineStr">
@@ -5311,7 +5305,7 @@
       <c r="A135" t="n">
         <v>134</v>
       </c>
-      <c r="B135" s="8" t="n">
+      <c r="B135" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C135" t="inlineStr">
@@ -5347,7 +5341,7 @@
       <c r="A136" t="n">
         <v>135</v>
       </c>
-      <c r="B136" s="8" t="n">
+      <c r="B136" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C136" t="inlineStr">
@@ -5383,7 +5377,7 @@
       <c r="A137" t="n">
         <v>136</v>
       </c>
-      <c r="B137" s="8" t="n">
+      <c r="B137" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C137" t="inlineStr">
@@ -5419,7 +5413,7 @@
       <c r="A138" t="n">
         <v>137</v>
       </c>
-      <c r="B138" s="8" t="n">
+      <c r="B138" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C138" t="inlineStr">
@@ -5455,7 +5449,7 @@
       <c r="A139" t="n">
         <v>138</v>
       </c>
-      <c r="B139" s="8" t="n">
+      <c r="B139" s="2" t="n">
         <v>45872</v>
       </c>
       <c r="C139" t="inlineStr">
@@ -5491,7 +5485,7 @@
       <c r="A140" t="n">
         <v>139</v>
       </c>
-      <c r="B140" s="8" t="n">
+      <c r="B140" s="2" t="n">
         <v>45873</v>
       </c>
       <c r="C140" t="inlineStr">
@@ -5527,7 +5521,7 @@
       <c r="A141" t="n">
         <v>140</v>
       </c>
-      <c r="B141" s="8" t="n">
+      <c r="B141" s="2" t="n">
         <v>45873</v>
       </c>
       <c r="C141" t="inlineStr">
@@ -5563,7 +5557,7 @@
       <c r="A142" t="n">
         <v>141</v>
       </c>
-      <c r="B142" s="8" t="n">
+      <c r="B142" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="C142" t="inlineStr">
@@ -5599,7 +5593,7 @@
       <c r="A143" t="n">
         <v>142</v>
       </c>
-      <c r="B143" s="8" t="n">
+      <c r="B143" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C143" t="inlineStr">
@@ -5635,7 +5629,7 @@
       <c r="A144" t="n">
         <v>143</v>
       </c>
-      <c r="B144" s="8" t="n">
+      <c r="B144" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C144" t="inlineStr">
@@ -5671,7 +5665,7 @@
       <c r="A145" t="n">
         <v>144</v>
       </c>
-      <c r="B145" s="8" t="n">
+      <c r="B145" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C145" t="inlineStr">
@@ -5707,7 +5701,7 @@
       <c r="A146" t="n">
         <v>145</v>
       </c>
-      <c r="B146" s="8" t="n">
+      <c r="B146" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C146" t="inlineStr">
@@ -5743,7 +5737,7 @@
       <c r="A147" t="n">
         <v>146</v>
       </c>
-      <c r="B147" s="8" t="n">
+      <c r="B147" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="C147" t="inlineStr">
@@ -5779,7 +5773,7 @@
       <c r="A148" t="n">
         <v>147</v>
       </c>
-      <c r="B148" s="8" t="n">
+      <c r="B148" s="2" t="n">
         <v>45860</v>
       </c>
       <c r="C148" t="inlineStr">
@@ -5815,7 +5809,7 @@
       <c r="A149" t="n">
         <v>148</v>
       </c>
-      <c r="B149" s="8" t="n">
+      <c r="B149" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C149" t="inlineStr">
@@ -5851,7 +5845,7 @@
       <c r="A150" t="n">
         <v>149</v>
       </c>
-      <c r="B150" s="8" t="n">
+      <c r="B150" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C150" t="inlineStr">
@@ -5887,7 +5881,7 @@
       <c r="A151" t="n">
         <v>150</v>
       </c>
-      <c r="B151" s="8" t="n">
+      <c r="B151" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C151" t="inlineStr">
@@ -5923,7 +5917,7 @@
       <c r="A152" t="n">
         <v>151</v>
       </c>
-      <c r="B152" s="8" t="n">
+      <c r="B152" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C152" t="inlineStr">
@@ -5959,7 +5953,7 @@
       <c r="A153" t="n">
         <v>152</v>
       </c>
-      <c r="B153" s="8" t="n">
+      <c r="B153" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C153" t="inlineStr">
@@ -5995,7 +5989,7 @@
       <c r="A154" t="n">
         <v>153</v>
       </c>
-      <c r="B154" s="8" t="n">
+      <c r="B154" s="2" t="n">
         <v>45890</v>
       </c>
       <c r="C154" t="inlineStr">
@@ -6031,7 +6025,7 @@
       <c r="A155" t="n">
         <v>154</v>
       </c>
-      <c r="B155" s="8" t="n">
+      <c r="B155" s="2" t="n">
         <v>45890</v>
       </c>
       <c r="C155" t="inlineStr">
@@ -6067,7 +6061,7 @@
       <c r="A156" t="n">
         <v>155</v>
       </c>
-      <c r="B156" s="8" t="n">
+      <c r="B156" s="2" t="n">
         <v>45897</v>
       </c>
       <c r="C156" t="inlineStr">
@@ -6103,7 +6097,7 @@
       <c r="A157" t="n">
         <v>156</v>
       </c>
-      <c r="B157" s="8" t="n">
+      <c r="B157" s="2" t="n">
         <v>45897</v>
       </c>
       <c r="C157" t="inlineStr">
@@ -6139,7 +6133,7 @@
       <c r="A158" t="n">
         <v>157</v>
       </c>
-      <c r="B158" s="8" t="n">
+      <c r="B158" s="2" t="n">
         <v>45897</v>
       </c>
       <c r="C158" t="inlineStr">
@@ -6175,7 +6169,7 @@
       <c r="A159" t="n">
         <v>158</v>
       </c>
-      <c r="B159" s="8" t="n">
+      <c r="B159" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C159" t="inlineStr">
@@ -6211,7 +6205,7 @@
       <c r="A160" t="n">
         <v>159</v>
       </c>
-      <c r="B160" s="8" t="n">
+      <c r="B160" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C160" t="inlineStr">
@@ -6247,7 +6241,7 @@
       <c r="A161" t="n">
         <v>160</v>
       </c>
-      <c r="B161" s="8" t="n">
+      <c r="B161" s="2" t="n">
         <v>45914</v>
       </c>
       <c r="C161" t="inlineStr">
@@ -6283,7 +6277,7 @@
       <c r="A162" t="n">
         <v>161</v>
       </c>
-      <c r="B162" s="8" t="n">
+      <c r="B162" s="2" t="n">
         <v>45890</v>
       </c>
       <c r="C162" t="inlineStr">
@@ -6319,7 +6313,7 @@
       <c r="A163" t="n">
         <v>162</v>
       </c>
-      <c r="B163" s="8" t="n">
+      <c r="B163" s="2" t="n">
         <v>45890</v>
       </c>
       <c r="C163" t="inlineStr">
@@ -6355,7 +6349,7 @@
       <c r="A164" t="n">
         <v>163</v>
       </c>
-      <c r="B164" s="8" t="n">
+      <c r="B164" s="2" t="n">
         <v>45896</v>
       </c>
       <c r="C164" t="inlineStr">
@@ -6391,7 +6385,7 @@
       <c r="A165" t="n">
         <v>164</v>
       </c>
-      <c r="B165" s="8" t="n">
+      <c r="B165" s="2" t="n">
         <v>45904</v>
       </c>
       <c r="C165" t="inlineStr">
@@ -6427,7 +6421,7 @@
       <c r="A166" t="n">
         <v>165</v>
       </c>
-      <c r="B166" s="8" t="n">
+      <c r="B166" s="2" t="n">
         <v>45879</v>
       </c>
       <c r="C166" t="inlineStr">
@@ -6463,7 +6457,7 @@
       <c r="A167" t="n">
         <v>166</v>
       </c>
-      <c r="B167" s="8" t="n">
+      <c r="B167" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C167" t="inlineStr">
@@ -6499,7 +6493,7 @@
       <c r="A168" t="n">
         <v>167</v>
       </c>
-      <c r="B168" s="8" t="n">
+      <c r="B168" s="2" t="n">
         <v>45881</v>
       </c>
       <c r="C168" t="inlineStr">
@@ -6535,7 +6529,7 @@
       <c r="A169" t="n">
         <v>168</v>
       </c>
-      <c r="B169" s="8" t="n">
+      <c r="B169" s="2" t="n">
         <v>45888</v>
       </c>
       <c r="C169" t="inlineStr">
@@ -6571,7 +6565,7 @@
       <c r="A170" t="n">
         <v>169</v>
       </c>
-      <c r="B170" s="8" t="n">
+      <c r="B170" s="2" t="n">
         <v>45889</v>
       </c>
       <c r="C170" t="inlineStr">
@@ -6607,7 +6601,7 @@
       <c r="A171" t="n">
         <v>170</v>
       </c>
-      <c r="B171" s="8" t="n">
+      <c r="B171" s="2" t="n">
         <v>45890</v>
       </c>
       <c r="C171" t="inlineStr">
@@ -6643,7 +6637,7 @@
       <c r="A172" t="n">
         <v>171</v>
       </c>
-      <c r="B172" s="8" t="n">
+      <c r="B172" s="2" t="n">
         <v>45895</v>
       </c>
       <c r="C172" t="inlineStr">
@@ -6679,7 +6673,7 @@
       <c r="A173" t="n">
         <v>172</v>
       </c>
-      <c r="B173" s="8" t="n">
+      <c r="B173" s="2" t="n">
         <v>45895</v>
       </c>
       <c r="C173" t="inlineStr">
@@ -6715,7 +6709,7 @@
       <c r="A174" t="n">
         <v>173</v>
       </c>
-      <c r="B174" s="8" t="n">
+      <c r="B174" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="C174" t="inlineStr">
@@ -6751,7 +6745,7 @@
       <c r="A175" t="n">
         <v>174</v>
       </c>
-      <c r="B175" s="8" t="n">
+      <c r="B175" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="C175" t="inlineStr">
@@ -6787,7 +6781,7 @@
       <c r="A176" t="n">
         <v>175</v>
       </c>
-      <c r="B176" s="8" t="n">
+      <c r="B176" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="C176" t="inlineStr">
@@ -6823,7 +6817,7 @@
       <c r="A177" t="n">
         <v>176</v>
       </c>
-      <c r="B177" s="8" t="n">
+      <c r="B177" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="C177" t="inlineStr">
@@ -6859,7 +6853,7 @@
       <c r="A178" t="n">
         <v>177</v>
       </c>
-      <c r="B178" s="8" t="n">
+      <c r="B178" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="C178" t="inlineStr">
@@ -6895,7 +6889,7 @@
       <c r="A179" t="n">
         <v>178</v>
       </c>
-      <c r="B179" s="8" t="n">
+      <c r="B179" s="2" t="n">
         <v>45881</v>
       </c>
       <c r="C179" t="inlineStr">
@@ -6931,7 +6925,7 @@
       <c r="A180" t="n">
         <v>179</v>
       </c>
-      <c r="B180" s="8" t="n">
+      <c r="B180" s="2" t="n">
         <v>45885</v>
       </c>
       <c r="C180" t="inlineStr">
@@ -6967,7 +6961,7 @@
       <c r="A181" t="n">
         <v>180</v>
       </c>
-      <c r="B181" s="8" t="n">
+      <c r="B181" s="2" t="n">
         <v>45856</v>
       </c>
       <c r="C181" t="inlineStr">
@@ -7003,7 +6997,7 @@
       <c r="A182" t="n">
         <v>181</v>
       </c>
-      <c r="B182" s="8" t="n">
+      <c r="B182" s="2" t="n">
         <v>45879</v>
       </c>
       <c r="C182" t="inlineStr">
@@ -7039,7 +7033,7 @@
       <c r="A183" t="n">
         <v>182</v>
       </c>
-      <c r="B183" s="8" t="n">
+      <c r="B183" s="2" t="n">
         <v>45886</v>
       </c>
       <c r="C183" t="inlineStr">
@@ -7075,7 +7069,7 @@
       <c r="A184" t="n">
         <v>183</v>
       </c>
-      <c r="B184" s="8" t="n">
+      <c r="B184" s="2" t="n">
         <v>45885</v>
       </c>
       <c r="C184" t="inlineStr">
@@ -7111,7 +7105,7 @@
       <c r="A185" t="n">
         <v>184</v>
       </c>
-      <c r="B185" s="8" t="n">
+      <c r="B185" s="2" t="n">
         <v>45901</v>
       </c>
       <c r="C185" t="inlineStr">
@@ -7147,7 +7141,7 @@
       <c r="A186" t="n">
         <v>185</v>
       </c>
-      <c r="B186" s="8" t="n">
+      <c r="B186" s="2" t="n">
         <v>45855</v>
       </c>
       <c r="C186" t="inlineStr">
@@ -7183,7 +7177,7 @@
       <c r="A187" t="n">
         <v>186</v>
       </c>
-      <c r="B187" s="8" t="n">
+      <c r="B187" s="2" t="n">
         <v>45885</v>
       </c>
       <c r="C187" t="inlineStr">
@@ -7219,7 +7213,7 @@
       <c r="A188" t="n">
         <v>187</v>
       </c>
-      <c r="B188" s="8" t="n">
+      <c r="B188" s="2" t="n">
         <v>45888</v>
       </c>
       <c r="C188" t="inlineStr">
@@ -7255,7 +7249,7 @@
       <c r="A189" t="n">
         <v>188</v>
       </c>
-      <c r="B189" s="8" t="n">
+      <c r="B189" s="2" t="n">
         <v>45889</v>
       </c>
       <c r="C189" t="inlineStr">
@@ -7291,7 +7285,7 @@
       <c r="A190" t="n">
         <v>189</v>
       </c>
-      <c r="B190" s="8" t="n">
+      <c r="B190" s="2" t="n">
         <v>45892</v>
       </c>
       <c r="C190" t="inlineStr">
@@ -7327,7 +7321,7 @@
       <c r="A191" t="n">
         <v>190</v>
       </c>
-      <c r="B191" s="8" t="n">
+      <c r="B191" s="2" t="n">
         <v>45855</v>
       </c>
       <c r="C191" t="inlineStr">
@@ -7363,7 +7357,7 @@
       <c r="A192" t="n">
         <v>191</v>
       </c>
-      <c r="B192" s="8" t="n">
+      <c r="B192" s="2" t="n">
         <v>45855</v>
       </c>
       <c r="C192" t="inlineStr">
@@ -7399,7 +7393,7 @@
       <c r="A193" t="n">
         <v>192</v>
       </c>
-      <c r="B193" s="8" t="n">
+      <c r="B193" s="2" t="n">
         <v>45855</v>
       </c>
       <c r="C193" t="inlineStr">
@@ -7435,7 +7429,7 @@
       <c r="A194" t="n">
         <v>193</v>
       </c>
-      <c r="B194" s="8" t="n">
+      <c r="B194" s="2" t="n">
         <v>45896</v>
       </c>
       <c r="C194" t="inlineStr">
@@ -7471,7 +7465,7 @@
       <c r="A195" t="n">
         <v>194</v>
       </c>
-      <c r="B195" s="8" t="n">
+      <c r="B195" s="2" t="n">
         <v>45901</v>
       </c>
       <c r="C195" t="inlineStr">
@@ -7507,7 +7501,7 @@
       <c r="A196" t="n">
         <v>195</v>
       </c>
-      <c r="B196" s="8" t="n">
+      <c r="B196" s="2" t="n">
         <v>45905</v>
       </c>
       <c r="C196" t="inlineStr">
@@ -7543,7 +7537,7 @@
       <c r="A197" t="n">
         <v>196</v>
       </c>
-      <c r="B197" s="8" t="n">
+      <c r="B197" s="2" t="n">
         <v>45905</v>
       </c>
       <c r="C197" t="inlineStr">
@@ -7579,7 +7573,7 @@
       <c r="A198" t="n">
         <v>197</v>
       </c>
-      <c r="B198" s="8" t="n">
+      <c r="B198" s="2" t="n">
         <v>45905</v>
       </c>
       <c r="C198" t="inlineStr">
@@ -7615,7 +7609,7 @@
       <c r="A199" t="n">
         <v>198</v>
       </c>
-      <c r="B199" s="8" t="n">
+      <c r="B199" s="2" t="n">
         <v>45905</v>
       </c>
       <c r="C199" t="inlineStr">
@@ -7651,7 +7645,7 @@
       <c r="A200" t="n">
         <v>199</v>
       </c>
-      <c r="B200" s="8" t="n">
+      <c r="B200" s="2" t="n">
         <v>45905</v>
       </c>
       <c r="C200" t="inlineStr">
@@ -7687,7 +7681,7 @@
       <c r="A201" t="n">
         <v>200</v>
       </c>
-      <c r="B201" s="8" t="n">
+      <c r="B201" s="2" t="n">
         <v>45905</v>
       </c>
       <c r="C201" t="inlineStr">
@@ -7723,7 +7717,7 @@
       <c r="A202" t="n">
         <v>201</v>
       </c>
-      <c r="B202" s="8" t="n">
+      <c r="B202" s="2" t="n">
         <v>45905</v>
       </c>
       <c r="C202" t="inlineStr">
@@ -7759,7 +7753,7 @@
       <c r="A203" t="n">
         <v>202</v>
       </c>
-      <c r="B203" s="8" t="n">
+      <c r="B203" s="2" t="n">
         <v>45906</v>
       </c>
       <c r="C203" t="inlineStr">
@@ -7795,7 +7789,7 @@
       <c r="A204" t="n">
         <v>203</v>
       </c>
-      <c r="B204" s="8" t="n">
+      <c r="B204" s="2" t="n">
         <v>45909</v>
       </c>
       <c r="C204" t="inlineStr">
@@ -7831,7 +7825,7 @@
       <c r="A205" t="n">
         <v>204</v>
       </c>
-      <c r="B205" s="8" t="n">
+      <c r="B205" s="2" t="n">
         <v>45910</v>
       </c>
       <c r="C205" t="inlineStr">
@@ -7867,7 +7861,7 @@
       <c r="A206" t="n">
         <v>205</v>
       </c>
-      <c r="B206" s="8" t="n">
+      <c r="B206" s="2" t="n">
         <v>45909</v>
       </c>
       <c r="C206" t="inlineStr">
@@ -7903,7 +7897,7 @@
       <c r="A207" t="n">
         <v>206</v>
       </c>
-      <c r="B207" s="8" t="n">
+      <c r="B207" s="2" t="n">
         <v>45909</v>
       </c>
       <c r="C207" t="inlineStr">
@@ -7939,7 +7933,7 @@
       <c r="A208" t="n">
         <v>207</v>
       </c>
-      <c r="B208" s="8" t="n">
+      <c r="B208" s="2" t="n">
         <v>45910</v>
       </c>
       <c r="C208" t="inlineStr">
@@ -7975,7 +7969,7 @@
       <c r="A209" t="n">
         <v>208</v>
       </c>
-      <c r="B209" s="8" t="n">
+      <c r="B209" s="2" t="n">
         <v>45878</v>
       </c>
       <c r="C209" t="inlineStr">
@@ -8011,7 +8005,7 @@
       <c r="A210" t="n">
         <v>209</v>
       </c>
-      <c r="B210" s="8" t="n">
+      <c r="B210" s="2" t="n">
         <v>45878</v>
       </c>
       <c r="C210" t="inlineStr">
@@ -8047,7 +8041,7 @@
       <c r="A211" t="n">
         <v>210</v>
       </c>
-      <c r="B211" s="8" t="n">
+      <c r="B211" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C211" t="inlineStr">
@@ -8083,7 +8077,7 @@
       <c r="A212" t="n">
         <v>211</v>
       </c>
-      <c r="B212" s="8" t="n">
+      <c r="B212" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C212" t="inlineStr">
@@ -8119,7 +8113,7 @@
       <c r="A213" t="n">
         <v>212</v>
       </c>
-      <c r="B213" s="8" t="n">
+      <c r="B213" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C213" t="inlineStr">
@@ -8155,7 +8149,7 @@
       <c r="A214" t="n">
         <v>213</v>
       </c>
-      <c r="B214" s="8" t="n">
+      <c r="B214" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C214" t="inlineStr">
@@ -8191,7 +8185,7 @@
       <c r="A215" t="n">
         <v>214</v>
       </c>
-      <c r="B215" s="8" t="n">
+      <c r="B215" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C215" t="inlineStr">
@@ -8227,7 +8221,7 @@
       <c r="A216" t="n">
         <v>215</v>
       </c>
-      <c r="B216" s="8" t="n">
+      <c r="B216" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C216" t="inlineStr">
@@ -8263,7 +8257,7 @@
       <c r="A217" t="n">
         <v>216</v>
       </c>
-      <c r="B217" s="8" t="n">
+      <c r="B217" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C217" t="inlineStr">
@@ -8299,7 +8293,7 @@
       <c r="A218" t="n">
         <v>217</v>
       </c>
-      <c r="B218" s="8" t="n">
+      <c r="B218" s="2" t="n">
         <v>45910</v>
       </c>
       <c r="C218" t="inlineStr">
@@ -8335,7 +8329,7 @@
       <c r="A219" t="n">
         <v>218</v>
       </c>
-      <c r="B219" s="8" t="n">
+      <c r="B219" s="2" t="n">
         <v>45910</v>
       </c>
       <c r="C219" t="inlineStr">
@@ -8371,7 +8365,7 @@
       <c r="A220" t="n">
         <v>219</v>
       </c>
-      <c r="B220" s="8" t="n">
+      <c r="B220" s="2" t="n">
         <v>45909</v>
       </c>
       <c r="C220" t="inlineStr">
@@ -8407,7 +8401,7 @@
       <c r="A221" t="n">
         <v>220</v>
       </c>
-      <c r="B221" s="8" t="n">
+      <c r="B221" s="2" t="n">
         <v>45909</v>
       </c>
       <c r="C221" t="inlineStr">
@@ -8443,7 +8437,7 @@
       <c r="A222" t="n">
         <v>221</v>
       </c>
-      <c r="B222" s="8" t="n">
+      <c r="B222" s="2" t="n">
         <v>45910</v>
       </c>
       <c r="C222" t="inlineStr">
@@ -8479,7 +8473,7 @@
       <c r="A223" t="n">
         <v>222</v>
       </c>
-      <c r="B223" s="8" t="n">
+      <c r="B223" s="2" t="n">
         <v>45890</v>
       </c>
       <c r="C223" t="inlineStr">
@@ -8515,7 +8509,7 @@
       <c r="A224" t="n">
         <v>223</v>
       </c>
-      <c r="B224" s="8" t="n">
+      <c r="B224" s="2" t="n">
         <v>45890</v>
       </c>
       <c r="C224" t="inlineStr">
@@ -8551,7 +8545,7 @@
       <c r="A225" t="n">
         <v>224</v>
       </c>
-      <c r="B225" s="8" t="n">
+      <c r="B225" s="2" t="n">
         <v>45898</v>
       </c>
       <c r="C225" t="inlineStr">
@@ -8587,7 +8581,7 @@
       <c r="A226" t="n">
         <v>225</v>
       </c>
-      <c r="B226" s="8" t="n">
+      <c r="B226" s="2" t="n">
         <v>45930</v>
       </c>
       <c r="C226" t="inlineStr">
@@ -8623,7 +8617,7 @@
       <c r="A227" t="n">
         <v>226</v>
       </c>
-      <c r="B227" s="8" t="n">
+      <c r="B227" s="2" t="n">
         <v>45911</v>
       </c>
       <c r="C227" t="inlineStr">
@@ -8659,7 +8653,7 @@
       <c r="A228" t="n">
         <v>227</v>
       </c>
-      <c r="B228" s="8" t="n">
+      <c r="B228" s="2" t="n">
         <v>45883</v>
       </c>
       <c r="C228" t="inlineStr">
@@ -8695,7 +8689,7 @@
       <c r="A229" t="n">
         <v>228</v>
       </c>
-      <c r="B229" s="8" t="n">
+      <c r="B229" s="2" t="n">
         <v>45890</v>
       </c>
       <c r="C229" t="inlineStr">
@@ -8731,7 +8725,7 @@
       <c r="A230" t="n">
         <v>229</v>
       </c>
-      <c r="B230" s="8" t="n">
+      <c r="B230" s="2" t="n">
         <v>45879</v>
       </c>
       <c r="C230" t="inlineStr">
@@ -8767,7 +8761,7 @@
       <c r="A231" t="n">
         <v>230</v>
       </c>
-      <c r="B231" s="8" t="n">
+      <c r="B231" s="2" t="n">
         <v>45892</v>
       </c>
       <c r="C231" t="inlineStr">
@@ -8803,7 +8797,7 @@
       <c r="A232" t="n">
         <v>231</v>
       </c>
-      <c r="B232" s="8" t="n">
+      <c r="B232" s="2" t="n">
         <v>45896</v>
       </c>
       <c r="C232" t="inlineStr">
@@ -8839,7 +8833,7 @@
       <c r="A233" t="n">
         <v>232</v>
       </c>
-      <c r="B233" s="8" t="n">
+      <c r="B233" s="2" t="n">
         <v>45893</v>
       </c>
       <c r="C233" t="inlineStr">
@@ -8875,7 +8869,7 @@
       <c r="A234" t="n">
         <v>233</v>
       </c>
-      <c r="B234" s="8" t="n">
+      <c r="B234" s="2" t="n">
         <v>45927</v>
       </c>
       <c r="C234" t="inlineStr">
@@ -8911,7 +8905,7 @@
       <c r="A235" t="n">
         <v>234</v>
       </c>
-      <c r="B235" s="8" t="n">
+      <c r="B235" s="2" t="n">
         <v>45896</v>
       </c>
       <c r="C235" t="inlineStr">
@@ -8947,7 +8941,7 @@
       <c r="A236" t="n">
         <v>235</v>
       </c>
-      <c r="B236" s="8" t="n">
+      <c r="B236" s="2" t="n">
         <v>45912</v>
       </c>
       <c r="C236" t="inlineStr">
@@ -8983,7 +8977,7 @@
       <c r="A237" t="n">
         <v>236</v>
       </c>
-      <c r="B237" s="8" t="n">
+      <c r="B237" s="2" t="n">
         <v>45912</v>
       </c>
       <c r="C237" t="inlineStr">
@@ -9019,7 +9013,7 @@
       <c r="A238" t="n">
         <v>237</v>
       </c>
-      <c r="B238" s="8" t="n">
+      <c r="B238" s="2" t="n">
         <v>45913</v>
       </c>
       <c r="C238" t="inlineStr">
@@ -9055,7 +9049,7 @@
       <c r="A239" t="n">
         <v>238</v>
       </c>
-      <c r="B239" s="8" t="n">
+      <c r="B239" s="2" t="n">
         <v>45914</v>
       </c>
       <c r="C239" t="inlineStr">
@@ -9091,7 +9085,7 @@
       <c r="A240" t="n">
         <v>239</v>
       </c>
-      <c r="B240" s="8" t="n">
+      <c r="B240" s="2" t="n">
         <v>45916</v>
       </c>
       <c r="C240" t="inlineStr">
@@ -9127,7 +9121,7 @@
       <c r="A241" t="n">
         <v>240</v>
       </c>
-      <c r="B241" s="8" t="n">
+      <c r="B241" s="2" t="n">
         <v>45916</v>
       </c>
       <c r="C241" t="inlineStr">
@@ -9163,7 +9157,7 @@
       <c r="A242" t="n">
         <v>241</v>
       </c>
-      <c r="B242" s="8" t="n">
+      <c r="B242" s="2" t="n">
         <v>45921</v>
       </c>
       <c r="C242" t="inlineStr">
@@ -9199,7 +9193,7 @@
       <c r="A243" t="n">
         <v>242</v>
       </c>
-      <c r="B243" s="8" t="n">
+      <c r="B243" s="2" t="n">
         <v>45920</v>
       </c>
       <c r="C243" t="inlineStr">
@@ -9235,7 +9229,7 @@
       <c r="A244" t="n">
         <v>243</v>
       </c>
-      <c r="B244" s="8" t="n">
+      <c r="B244" s="2" t="n">
         <v>45921</v>
       </c>
       <c r="C244" t="inlineStr">
@@ -9271,7 +9265,7 @@
       <c r="A245" t="n">
         <v>244</v>
       </c>
-      <c r="B245" s="9" t="n">
+      <c r="B245" s="3" t="n">
         <v>45922</v>
       </c>
       <c r="C245" t="inlineStr">
@@ -9320,7 +9314,7 @@
       <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -9531,15 +9525,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col width="32.375" customWidth="1" style="6" min="2" max="2"/>
+    <col width="32.33203125" customWidth="1" style="1" min="2" max="2"/>
+    <col width="92.21875" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -9548,7 +9543,7 @@
           <t>Id</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Fecha</t>
         </is>
@@ -9588,7 +9583,7 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="n">
+      <c r="B2" s="4" t="n">
         <v>45880</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -9624,7 +9619,7 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="4" t="n">
         <v>45871</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -9660,7 +9655,7 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="4" t="n">
         <v>45871</v>
       </c>
       <c r="C4" t="inlineStr">
@@ -9696,7 +9691,7 @@
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="B5" s="4" t="n">
         <v>45872</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -9732,7 +9727,7 @@
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="4" t="n">
         <v>45877</v>
       </c>
       <c r="C6" t="inlineStr">
@@ -9768,7 +9763,7 @@
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="n">
+      <c r="B7" s="4" t="n">
         <v>45881</v>
       </c>
       <c r="C7" t="inlineStr">
@@ -9804,7 +9799,7 @@
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="n">
+      <c r="B8" s="4" t="n">
         <v>45922</v>
       </c>
       <c r="C8" t="inlineStr">
@@ -9840,7 +9835,7 @@
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="4" t="n">
         <v>45891</v>
       </c>
       <c r="C9" t="inlineStr">
@@ -9876,7 +9871,7 @@
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="n">
+      <c r="B10" s="4" t="n">
         <v>45899</v>
       </c>
       <c r="C10" t="inlineStr">
@@ -9912,7 +9907,7 @@
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="n">
+      <c r="B11" s="4" t="n">
         <v>45870</v>
       </c>
       <c r="C11" t="inlineStr">
@@ -9948,7 +9943,7 @@
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="4" t="n">
         <v>45876</v>
       </c>
       <c r="C12" t="inlineStr">
@@ -9984,7 +9979,7 @@
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="4" t="n">
         <v>45875</v>
       </c>
       <c r="C13" t="inlineStr">
@@ -10020,7 +10015,7 @@
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="n">
+      <c r="B14" s="4" t="n">
         <v>45877</v>
       </c>
       <c r="C14" t="inlineStr">
@@ -10056,7 +10051,7 @@
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="n">
+      <c r="B15" s="4" t="n">
         <v>45881</v>
       </c>
       <c r="C15" t="inlineStr">
@@ -10092,7 +10087,7 @@
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="n">
+      <c r="B16" s="4" t="n">
         <v>45884</v>
       </c>
       <c r="C16" t="inlineStr">
@@ -10128,7 +10123,7 @@
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="n">
+      <c r="B17" s="4" t="n">
         <v>45887</v>
       </c>
       <c r="C17" t="inlineStr">
@@ -10164,7 +10159,7 @@
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="n">
+      <c r="B18" s="4" t="n">
         <v>45887</v>
       </c>
       <c r="C18" t="inlineStr">
@@ -10200,7 +10195,7 @@
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="n">
+      <c r="B19" s="4" t="n">
         <v>45898</v>
       </c>
       <c r="C19" t="inlineStr">
@@ -10236,7 +10231,7 @@
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="n">
+      <c r="B20" s="4" t="n">
         <v>45891</v>
       </c>
       <c r="C20" t="inlineStr">
@@ -10272,7 +10267,7 @@
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="n">
+      <c r="B21" s="4" t="n">
         <v>45891</v>
       </c>
       <c r="C21" t="inlineStr">
@@ -10308,7 +10303,7 @@
       <c r="A22" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="n">
+      <c r="B22" s="4" t="n">
         <v>45901</v>
       </c>
       <c r="C22" t="inlineStr">
@@ -10344,7 +10339,7 @@
       <c r="A23" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="n">
+      <c r="B23" s="4" t="n">
         <v>45868</v>
       </c>
       <c r="C23" t="inlineStr">
@@ -10380,7 +10375,7 @@
       <c r="A24" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="n">
+      <c r="B24" s="4" t="n">
         <v>45876</v>
       </c>
       <c r="C24" t="inlineStr">
@@ -10416,7 +10411,7 @@
       <c r="A25" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="n">
+      <c r="B25" s="4" t="n">
         <v>45882</v>
       </c>
       <c r="C25" t="inlineStr">
@@ -10452,7 +10447,7 @@
       <c r="A26" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="n">
+      <c r="B26" s="4" t="n">
         <v>45919</v>
       </c>
       <c r="C26" t="inlineStr">
@@ -10488,7 +10483,7 @@
       <c r="A27" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="n">
+      <c r="B27" s="4" t="n">
         <v>45907</v>
       </c>
       <c r="C27" t="inlineStr">
@@ -10524,7 +10519,7 @@
       <c r="A28" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="n">
+      <c r="B28" s="4" t="n">
         <v>45832</v>
       </c>
       <c r="C28" t="inlineStr">
@@ -10560,7 +10555,7 @@
       <c r="A29" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="n">
+      <c r="B29" s="4" t="n">
         <v>45836</v>
       </c>
       <c r="C29" t="inlineStr">
@@ -10596,7 +10591,7 @@
       <c r="A30" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="n">
+      <c r="B30" s="4" t="n">
         <v>45839</v>
       </c>
       <c r="C30" t="inlineStr">
@@ -10632,7 +10627,7 @@
       <c r="A31" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="n">
+      <c r="B31" s="4" t="n">
         <v>45839</v>
       </c>
       <c r="C31" t="inlineStr">
@@ -10668,7 +10663,7 @@
       <c r="A32" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="n">
+      <c r="B32" s="4" t="n">
         <v>45846</v>
       </c>
       <c r="C32" t="inlineStr">
@@ -10704,7 +10699,7 @@
       <c r="A33" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="n">
+      <c r="B33" s="4" t="n">
         <v>45842</v>
       </c>
       <c r="C33" t="inlineStr">
@@ -10740,7 +10735,7 @@
       <c r="A34" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="n">
+      <c r="B34" s="4" t="n">
         <v>45845</v>
       </c>
       <c r="C34" t="inlineStr">
@@ -10776,7 +10771,7 @@
       <c r="A35" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="n">
+      <c r="B35" s="4" t="n">
         <v>45850</v>
       </c>
       <c r="C35" t="inlineStr">
@@ -10812,7 +10807,7 @@
       <c r="A36" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="n">
+      <c r="B36" s="4" t="n">
         <v>45850</v>
       </c>
       <c r="C36" t="inlineStr">
@@ -10848,7 +10843,7 @@
       <c r="A37" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="8" t="n">
+      <c r="B37" s="4" t="n">
         <v>45863</v>
       </c>
       <c r="C37" t="inlineStr">
@@ -10884,7 +10879,7 @@
       <c r="A38" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="n">
+      <c r="B38" s="4" t="n">
         <v>45863</v>
       </c>
       <c r="C38" t="inlineStr">
@@ -10920,7 +10915,7 @@
       <c r="A39" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="n">
+      <c r="B39" s="4" t="n">
         <v>45866</v>
       </c>
       <c r="C39" t="inlineStr">
@@ -10956,7 +10951,7 @@
       <c r="A40" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="8" t="n">
+      <c r="B40" s="4" t="n">
         <v>45873</v>
       </c>
       <c r="C40" t="inlineStr">
@@ -10992,7 +10987,7 @@
       <c r="A41" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="8" t="n">
+      <c r="B41" s="4" t="n">
         <v>45790</v>
       </c>
       <c r="C41" t="inlineStr">
@@ -11028,7 +11023,7 @@
       <c r="A42" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="8" t="n">
+      <c r="B42" s="4" t="n">
         <v>45791</v>
       </c>
       <c r="C42" t="inlineStr">
@@ -11064,7 +11059,7 @@
       <c r="A43" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="8" t="n">
+      <c r="B43" s="4" t="n">
         <v>45793</v>
       </c>
       <c r="C43" t="inlineStr">
@@ -11100,7 +11095,7 @@
       <c r="A44" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="8" t="n">
+      <c r="B44" s="4" t="n">
         <v>45794</v>
       </c>
       <c r="C44" t="inlineStr">
@@ -11136,7 +11131,7 @@
       <c r="A45" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="8" t="n">
+      <c r="B45" s="4" t="n">
         <v>45797</v>
       </c>
       <c r="C45" t="inlineStr">
@@ -11172,7 +11167,7 @@
       <c r="A46" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="8" t="n">
+      <c r="B46" s="4" t="n">
         <v>45797</v>
       </c>
       <c r="C46" t="inlineStr">
@@ -11208,7 +11203,7 @@
       <c r="A47" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="8" t="n">
+      <c r="B47" s="4" t="n">
         <v>45797</v>
       </c>
       <c r="C47" t="inlineStr">
@@ -11244,7 +11239,7 @@
       <c r="A48" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="8" t="n">
+      <c r="B48" s="4" t="n">
         <v>45797</v>
       </c>
       <c r="C48" t="inlineStr">
@@ -11280,7 +11275,7 @@
       <c r="A49" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="8" t="n">
+      <c r="B49" s="4" t="n">
         <v>45806</v>
       </c>
       <c r="C49" t="inlineStr">
@@ -11316,7 +11311,7 @@
       <c r="A50" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="8" t="n">
+      <c r="B50" s="4" t="n">
         <v>45821</v>
       </c>
       <c r="C50" t="inlineStr">
@@ -11352,7 +11347,7 @@
       <c r="A51" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="8" t="n">
+      <c r="B51" s="4" t="n">
         <v>45821</v>
       </c>
       <c r="C51" t="inlineStr">
@@ -11388,7 +11383,7 @@
       <c r="A52" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="8" t="n">
+      <c r="B52" s="4" t="n">
         <v>45822</v>
       </c>
       <c r="C52" t="inlineStr">
@@ -11424,7 +11419,7 @@
       <c r="A53" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="8" t="n">
+      <c r="B53" s="4" t="n">
         <v>45822</v>
       </c>
       <c r="C53" t="inlineStr">
@@ -11460,7 +11455,7 @@
       <c r="A54" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="8" t="n">
+      <c r="B54" s="4" t="n">
         <v>45825</v>
       </c>
       <c r="C54" t="inlineStr">
@@ -11496,7 +11491,7 @@
       <c r="A55" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="8" t="n">
+      <c r="B55" s="4" t="n">
         <v>45826</v>
       </c>
       <c r="C55" t="inlineStr">
@@ -11532,7 +11527,7 @@
       <c r="A56" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="8" t="n">
+      <c r="B56" s="4" t="n">
         <v>45829</v>
       </c>
       <c r="C56" t="inlineStr">
@@ -11568,7 +11563,7 @@
       <c r="A57" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="8" t="n">
+      <c r="B57" s="4" t="n">
         <v>45843</v>
       </c>
       <c r="C57" t="inlineStr">
@@ -11604,7 +11599,7 @@
       <c r="A58" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="8" t="n">
+      <c r="B58" s="4" t="n">
         <v>45826</v>
       </c>
       <c r="C58" t="inlineStr">
@@ -11640,7 +11635,7 @@
       <c r="A59" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="8" t="n">
+      <c r="B59" s="4" t="n">
         <v>45828</v>
       </c>
       <c r="C59" t="inlineStr">
@@ -11676,7 +11671,7 @@
       <c r="A60" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="8" t="n">
+      <c r="B60" s="4" t="n">
         <v>45788</v>
       </c>
       <c r="C60" t="inlineStr">
@@ -11712,7 +11707,7 @@
       <c r="A61" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="8" t="n">
+      <c r="B61" s="4" t="n">
         <v>45848</v>
       </c>
       <c r="C61" t="inlineStr">
@@ -11748,7 +11743,7 @@
       <c r="A62" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="8" t="n">
+      <c r="B62" s="4" t="n">
         <v>45849</v>
       </c>
       <c r="C62" t="inlineStr">
@@ -11784,7 +11779,7 @@
       <c r="A63" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="8" t="n">
+      <c r="B63" s="4" t="n">
         <v>45877</v>
       </c>
       <c r="C63" t="inlineStr">
@@ -11820,7 +11815,7 @@
       <c r="A64" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="8" t="n">
+      <c r="B64" s="4" t="n">
         <v>45881</v>
       </c>
       <c r="C64" t="inlineStr">
@@ -11856,7 +11851,7 @@
       <c r="A65" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="8" t="n">
+      <c r="B65" s="4" t="n">
         <v>45892</v>
       </c>
       <c r="C65" t="inlineStr">
@@ -11892,7 +11887,7 @@
       <c r="A66" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="8" t="n">
+      <c r="B66" s="4" t="n">
         <v>45905</v>
       </c>
       <c r="C66" t="inlineStr">
@@ -11928,7 +11923,7 @@
       <c r="A67" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="8" t="n">
+      <c r="B67" s="4" t="n">
         <v>45886</v>
       </c>
       <c r="C67" t="inlineStr">
@@ -11964,7 +11959,7 @@
       <c r="A68" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="8" t="n">
+      <c r="B68" s="4" t="n">
         <v>45910</v>
       </c>
       <c r="C68" t="inlineStr">
@@ -12000,7 +11995,7 @@
       <c r="A69" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="8" t="n">
+      <c r="B69" s="4" t="n">
         <v>45898</v>
       </c>
       <c r="C69" t="inlineStr">
@@ -12036,7 +12031,7 @@
       <c r="A70" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="8" t="n">
+      <c r="B70" s="4" t="n">
         <v>45895</v>
       </c>
       <c r="C70" t="inlineStr">
@@ -12072,7 +12067,7 @@
       <c r="A71" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="8" t="n">
+      <c r="B71" s="4" t="n">
         <v>45902</v>
       </c>
       <c r="C71" t="inlineStr">
@@ -12108,7 +12103,7 @@
       <c r="A72" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="8" t="n">
+      <c r="B72" s="4" t="n">
         <v>45910</v>
       </c>
       <c r="C72" t="inlineStr">
@@ -12144,7 +12139,7 @@
       <c r="A73" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="8" t="n">
+      <c r="B73" s="4" t="n">
         <v>45910</v>
       </c>
       <c r="C73" t="inlineStr">
@@ -12180,7 +12175,7 @@
       <c r="A74" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="8" t="n">
+      <c r="B74" s="4" t="n">
         <v>45911</v>
       </c>
       <c r="C74" t="inlineStr">
@@ -12216,7 +12211,7 @@
       <c r="A75" t="n">
         <v>74</v>
       </c>
-      <c r="B75" s="8" t="n">
+      <c r="B75" s="4" t="n">
         <v>45893</v>
       </c>
       <c r="C75" t="inlineStr">
@@ -12252,7 +12247,7 @@
       <c r="A76" t="n">
         <v>75</v>
       </c>
-      <c r="B76" s="8" t="n">
+      <c r="B76" s="4" t="n">
         <v>45911</v>
       </c>
       <c r="C76" t="inlineStr">
@@ -12288,7 +12283,7 @@
       <c r="A77" t="n">
         <v>76</v>
       </c>
-      <c r="B77" s="8" t="n">
+      <c r="B77" s="4" t="n">
         <v>45914</v>
       </c>
       <c r="C77" t="inlineStr">
@@ -12324,7 +12319,7 @@
       <c r="A78" t="n">
         <v>77</v>
       </c>
-      <c r="B78" s="8" t="n">
+      <c r="B78" s="4" t="n">
         <v>45912</v>
       </c>
       <c r="C78" t="inlineStr">
@@ -12360,7 +12355,7 @@
       <c r="A79" t="n">
         <v>78</v>
       </c>
-      <c r="B79" s="8" t="n">
+      <c r="B79" s="4" t="n">
         <v>45919</v>
       </c>
       <c r="C79" t="inlineStr">
@@ -12396,7 +12391,7 @@
       <c r="A80" t="n">
         <v>79</v>
       </c>
-      <c r="B80" s="8" t="n">
+      <c r="B80" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C80" t="inlineStr">
@@ -12432,7 +12427,7 @@
       <c r="A81" t="n">
         <v>80</v>
       </c>
-      <c r="B81" s="8" t="n">
+      <c r="B81" s="4" t="n">
         <v>45899</v>
       </c>
       <c r="C81" t="inlineStr">
@@ -12468,7 +12463,7 @@
       <c r="A82" t="n">
         <v>81</v>
       </c>
-      <c r="B82" s="8" t="n">
+      <c r="B82" s="4" t="n">
         <v>45915</v>
       </c>
       <c r="C82" t="inlineStr">
@@ -12483,7 +12478,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Total 5 Res 101.6 x 205,000 : 20828000 + saldo anterior 329900 = total 21157900</t>
+          <t>5 Res 101.6 x 205,000 - la factura se realizo por : 20828000 + saldo anterior 329900 = total 21157900</t>
         </is>
       </c>
       <c r="F82" t="n">
@@ -12504,7 +12499,7 @@
       <c r="A83" t="n">
         <v>82</v>
       </c>
-      <c r="B83" s="8" t="n">
+      <c r="B83" s="4" t="n">
         <v>45902</v>
       </c>
       <c r="C83" t="inlineStr">
@@ -12540,7 +12535,7 @@
       <c r="A84" t="n">
         <v>83</v>
       </c>
-      <c r="B84" s="8" t="n">
+      <c r="B84" s="4" t="n">
         <v>45888</v>
       </c>
       <c r="C84" t="inlineStr">
@@ -12555,7 +12550,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Total 1 h 180x 190000 6 res 112088x205000 : 25714000 + saldo anterior 329900 = total 26043900</t>
+          <t>1 h 180x 190000 6 res 112088x205000 - la factura se realizo por : 25714000 + saldo anterior 329900 = total 26043900</t>
         </is>
       </c>
       <c r="F84" t="n">
@@ -12576,7 +12571,7 @@
       <c r="A85" t="n">
         <v>84</v>
       </c>
-      <c r="B85" s="8" t="n">
+      <c r="B85" s="4" t="n">
         <v>45905</v>
       </c>
       <c r="C85" t="inlineStr">
@@ -12612,7 +12607,7 @@
       <c r="A86" t="n">
         <v>85</v>
       </c>
-      <c r="B86" s="8" t="n">
+      <c r="B86" s="4" t="n">
         <v>45912</v>
       </c>
       <c r="C86" t="inlineStr">
@@ -12648,7 +12643,7 @@
       <c r="A87" t="n">
         <v>86</v>
       </c>
-      <c r="B87" s="9" t="n">
+      <c r="B87" s="4" t="n">
         <v>45908</v>
       </c>
       <c r="C87" t="inlineStr">
@@ -12663,11 +12658,11 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Total 3 Res aroba 5604 x212000 : 118804000 + saldo anterior -14956100 = total 103847900</t>
+          <t>3 Res aroba 5604 x212000 - la factura se realizo por : 10384790  + saldo anterior -14956100 = total -4571310</t>
         </is>
       </c>
       <c r="F87" t="n">
-        <v>103847900</v>
+        <v>-4571310</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -12680,8 +12675,262 @@
         </is>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" s="4" t="n">
+        <v>45923</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>100000</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" s="4" t="n">
+        <v>45924</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" s="4" t="n">
+        <v>45923</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" s="4" t="n">
+        <v>45925</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Factura - la factura se realizo por : 10000  + saldo anterior 90000 = total 100000</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>100000</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" s="4" t="n">
+        <v>45915</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" s="4" t="n">
+        <v>45910</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Factura - la factura se realizo por : 5000  + saldo anterior 90000 = total 95000</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>95000</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>F-003</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" s="4" t="n">
+        <v>45924</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>F-003</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H87"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -12691,13 +12940,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="22.77734375" customWidth="1" min="3" max="3"/>
+    <col width="23.33203125" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -12812,13 +13066,32 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>103847900</v>
+        <v>-4571310</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>103847900</v>
+        <v>-4571310</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>95000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E7" t="n">
+        <v>90000</v>
       </c>
     </row>
   </sheetData>
@@ -12834,13 +13107,13 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col width="16.875" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="16.88671875" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -12849,7 +13122,7 @@
           <t>Id</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Fecha</t>
         </is>
@@ -12879,7 +13152,7 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="1" t="n">
         <v>45908</v>
       </c>
       <c r="C2" t="inlineStr">

</xml_diff>

<commit_message>
Mejoras en presentacion de mensajes y paginacion
</commit_message>
<xml_diff>
--- a/FinancieroG.xlsx
+++ b/FinancieroG.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H245"/>
+  <dimension ref="A1:H253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
@@ -517,7 +517,7 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="4" t="n">
         <v>45816</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -553,7 +553,7 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="4" t="n">
         <v>45816</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -589,7 +589,7 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="4" t="n">
         <v>45818</v>
       </c>
       <c r="C4" t="inlineStr">
@@ -625,7 +625,7 @@
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="4" t="n">
         <v>45820</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -661,7 +661,7 @@
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="4" t="n">
         <v>45828</v>
       </c>
       <c r="C6" t="inlineStr">
@@ -697,7 +697,7 @@
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="4" t="n">
         <v>45843</v>
       </c>
       <c r="C7" t="inlineStr">
@@ -733,7 +733,7 @@
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="4" t="n">
         <v>45848</v>
       </c>
       <c r="C8" t="inlineStr">
@@ -769,7 +769,7 @@
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="4" t="n">
         <v>45849</v>
       </c>
       <c r="C9" t="inlineStr">
@@ -805,7 +805,7 @@
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="4" t="n">
         <v>45863</v>
       </c>
       <c r="C10" t="inlineStr">
@@ -841,7 +841,7 @@
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="4" t="n">
         <v>45807</v>
       </c>
       <c r="C11" t="inlineStr">
@@ -877,7 +877,7 @@
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="4" t="n">
         <v>45807</v>
       </c>
       <c r="C12" t="inlineStr">
@@ -913,7 +913,7 @@
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="4" t="n">
         <v>45722</v>
       </c>
       <c r="C13" t="inlineStr">
@@ -949,7 +949,7 @@
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="4" t="n">
         <v>45819</v>
       </c>
       <c r="C14" t="inlineStr">
@@ -985,7 +985,7 @@
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="4" t="n">
         <v>45820</v>
       </c>
       <c r="C15" t="inlineStr">
@@ -1021,7 +1021,7 @@
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="4" t="n">
         <v>45822</v>
       </c>
       <c r="C16" t="inlineStr">
@@ -1057,7 +1057,7 @@
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="4" t="n">
         <v>45822</v>
       </c>
       <c r="C17" t="inlineStr">
@@ -1093,7 +1093,7 @@
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="4" t="n">
         <v>45822</v>
       </c>
       <c r="C18" t="inlineStr">
@@ -1129,7 +1129,7 @@
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="4" t="n">
         <v>45829</v>
       </c>
       <c r="C19" t="inlineStr">
@@ -1165,7 +1165,7 @@
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="4" t="n">
         <v>45833</v>
       </c>
       <c r="C20" t="inlineStr">
@@ -1201,7 +1201,7 @@
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="4" t="n">
         <v>45836</v>
       </c>
       <c r="C21" t="inlineStr">
@@ -1237,7 +1237,7 @@
       <c r="A22" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="4" t="n">
         <v>45839</v>
       </c>
       <c r="C22" t="inlineStr">
@@ -1273,7 +1273,7 @@
       <c r="A23" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="4" t="n">
         <v>45839</v>
       </c>
       <c r="C23" t="inlineStr">
@@ -1309,7 +1309,7 @@
       <c r="A24" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="4" t="n">
         <v>45839</v>
       </c>
       <c r="C24" t="inlineStr">
@@ -1345,7 +1345,7 @@
       <c r="A25" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="4" t="n">
         <v>45839</v>
       </c>
       <c r="C25" t="inlineStr">
@@ -1381,7 +1381,7 @@
       <c r="A26" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="n">
+      <c r="B26" s="4" t="n">
         <v>45840</v>
       </c>
       <c r="C26" t="inlineStr">
@@ -1417,7 +1417,7 @@
       <c r="A27" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="4" t="n">
         <v>45840</v>
       </c>
       <c r="C27" t="inlineStr">
@@ -1453,7 +1453,7 @@
       <c r="A28" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="n">
+      <c r="B28" s="4" t="n">
         <v>45840</v>
       </c>
       <c r="C28" t="inlineStr">
@@ -1489,7 +1489,7 @@
       <c r="A29" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="n">
+      <c r="B29" s="4" t="n">
         <v>45841</v>
       </c>
       <c r="C29" t="inlineStr">
@@ -1525,7 +1525,7 @@
       <c r="A30" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="n">
+      <c r="B30" s="4" t="n">
         <v>45841</v>
       </c>
       <c r="C30" t="inlineStr">
@@ -1561,7 +1561,7 @@
       <c r="A31" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="n">
+      <c r="B31" s="4" t="n">
         <v>45841</v>
       </c>
       <c r="C31" t="inlineStr">
@@ -1597,7 +1597,7 @@
       <c r="A32" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="n">
+      <c r="B32" s="4" t="n">
         <v>45841</v>
       </c>
       <c r="C32" t="inlineStr">
@@ -1633,7 +1633,7 @@
       <c r="A33" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="n">
+      <c r="B33" s="4" t="n">
         <v>45841</v>
       </c>
       <c r="C33" t="inlineStr">
@@ -1669,7 +1669,7 @@
       <c r="A34" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="n">
+      <c r="B34" s="4" t="n">
         <v>45842</v>
       </c>
       <c r="C34" t="inlineStr">
@@ -1705,7 +1705,7 @@
       <c r="A35" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="n">
+      <c r="B35" s="4" t="n">
         <v>45847</v>
       </c>
       <c r="C35" t="inlineStr">
@@ -1741,7 +1741,7 @@
       <c r="A36" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="n">
+      <c r="B36" s="4" t="n">
         <v>45847</v>
       </c>
       <c r="C36" t="inlineStr">
@@ -1777,7 +1777,7 @@
       <c r="A37" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="n">
+      <c r="B37" s="4" t="n">
         <v>45847</v>
       </c>
       <c r="C37" t="inlineStr">
@@ -1813,7 +1813,7 @@
       <c r="A38" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="n">
+      <c r="B38" s="4" t="n">
         <v>45847</v>
       </c>
       <c r="C38" t="inlineStr">
@@ -1849,7 +1849,7 @@
       <c r="A39" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="n">
+      <c r="B39" s="4" t="n">
         <v>45847</v>
       </c>
       <c r="C39" t="inlineStr">
@@ -1885,7 +1885,7 @@
       <c r="A40" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="n">
+      <c r="B40" s="4" t="n">
         <v>45847</v>
       </c>
       <c r="C40" t="inlineStr">
@@ -1921,7 +1921,7 @@
       <c r="A41" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="n">
+      <c r="B41" s="4" t="n">
         <v>45847</v>
       </c>
       <c r="C41" t="inlineStr">
@@ -1957,7 +1957,7 @@
       <c r="A42" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="n">
+      <c r="B42" s="4" t="n">
         <v>45847</v>
       </c>
       <c r="C42" t="inlineStr">
@@ -1993,7 +1993,7 @@
       <c r="A43" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="n">
+      <c r="B43" s="4" t="n">
         <v>45850</v>
       </c>
       <c r="C43" t="inlineStr">
@@ -2029,7 +2029,7 @@
       <c r="A44" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="n">
+      <c r="B44" s="4" t="n">
         <v>45851</v>
       </c>
       <c r="C44" t="inlineStr">
@@ -2065,7 +2065,7 @@
       <c r="A45" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="2" t="n">
+      <c r="B45" s="4" t="n">
         <v>45861</v>
       </c>
       <c r="C45" t="inlineStr">
@@ -2101,7 +2101,7 @@
       <c r="A46" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="n">
+      <c r="B46" s="4" t="n">
         <v>45861</v>
       </c>
       <c r="C46" t="inlineStr">
@@ -2137,7 +2137,7 @@
       <c r="A47" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="2" t="n">
+      <c r="B47" s="4" t="n">
         <v>45861</v>
       </c>
       <c r="C47" t="inlineStr">
@@ -2173,7 +2173,7 @@
       <c r="A48" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="2" t="n">
+      <c r="B48" s="4" t="n">
         <v>45861</v>
       </c>
       <c r="C48" t="inlineStr">
@@ -2209,7 +2209,7 @@
       <c r="A49" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="n">
+      <c r="B49" s="4" t="n">
         <v>45870</v>
       </c>
       <c r="C49" t="inlineStr">
@@ -2245,7 +2245,7 @@
       <c r="A50" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="2" t="n">
+      <c r="B50" s="4" t="n">
         <v>45870</v>
       </c>
       <c r="C50" t="inlineStr">
@@ -2281,7 +2281,7 @@
       <c r="A51" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="2" t="n">
+      <c r="B51" s="4" t="n">
         <v>45873</v>
       </c>
       <c r="C51" t="inlineStr">
@@ -2317,7 +2317,7 @@
       <c r="A52" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="2" t="n">
+      <c r="B52" s="4" t="n">
         <v>45862</v>
       </c>
       <c r="C52" t="inlineStr">
@@ -2353,7 +2353,7 @@
       <c r="A53" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="2" t="n">
+      <c r="B53" s="4" t="n">
         <v>45864</v>
       </c>
       <c r="C53" t="inlineStr">
@@ -2389,7 +2389,7 @@
       <c r="A54" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="2" t="n">
+      <c r="B54" s="4" t="n">
         <v>45865</v>
       </c>
       <c r="C54" t="inlineStr">
@@ -2425,7 +2425,7 @@
       <c r="A55" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="2" t="n">
+      <c r="B55" s="4" t="n">
         <v>45863</v>
       </c>
       <c r="C55" t="inlineStr">
@@ -2461,7 +2461,7 @@
       <c r="A56" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="2" t="n">
+      <c r="B56" s="4" t="n">
         <v>45866</v>
       </c>
       <c r="C56" t="inlineStr">
@@ -2497,7 +2497,7 @@
       <c r="A57" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="2" t="n">
+      <c r="B57" s="4" t="n">
         <v>45870</v>
       </c>
       <c r="C57" t="inlineStr">
@@ -2533,7 +2533,7 @@
       <c r="A58" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="2" t="n">
+      <c r="B58" s="4" t="n">
         <v>45871</v>
       </c>
       <c r="C58" t="inlineStr">
@@ -2569,7 +2569,7 @@
       <c r="A59" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="2" t="n">
+      <c r="B59" s="4" t="n">
         <v>45871</v>
       </c>
       <c r="C59" t="inlineStr">
@@ -2605,7 +2605,7 @@
       <c r="A60" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="2" t="n">
+      <c r="B60" s="4" t="n">
         <v>45872</v>
       </c>
       <c r="C60" t="inlineStr">
@@ -2641,7 +2641,7 @@
       <c r="A61" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="2" t="n">
+      <c r="B61" s="4" t="n">
         <v>45828</v>
       </c>
       <c r="C61" t="inlineStr">
@@ -2677,7 +2677,7 @@
       <c r="A62" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="2" t="n">
+      <c r="B62" s="4" t="n">
         <v>45828</v>
       </c>
       <c r="C62" t="inlineStr">
@@ -2713,7 +2713,7 @@
       <c r="A63" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="2" t="n">
+      <c r="B63" s="4" t="n">
         <v>45832</v>
       </c>
       <c r="C63" t="inlineStr">
@@ -2749,7 +2749,7 @@
       <c r="A64" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="2" t="n">
+      <c r="B64" s="4" t="n">
         <v>45832</v>
       </c>
       <c r="C64" t="inlineStr">
@@ -2785,7 +2785,7 @@
       <c r="A65" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="2" t="n">
+      <c r="B65" s="4" t="n">
         <v>45820</v>
       </c>
       <c r="C65" t="inlineStr">
@@ -2821,7 +2821,7 @@
       <c r="A66" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="2" t="n">
+      <c r="B66" s="4" t="n">
         <v>45867</v>
       </c>
       <c r="C66" t="inlineStr">
@@ -2857,7 +2857,7 @@
       <c r="A67" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="2" t="n">
+      <c r="B67" s="4" t="n">
         <v>45867</v>
       </c>
       <c r="C67" t="inlineStr">
@@ -2893,7 +2893,7 @@
       <c r="A68" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="2" t="n">
+      <c r="B68" s="4" t="n">
         <v>45867</v>
       </c>
       <c r="C68" t="inlineStr">
@@ -2929,7 +2929,7 @@
       <c r="A69" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="2" t="n">
+      <c r="B69" s="4" t="n">
         <v>45867</v>
       </c>
       <c r="C69" t="inlineStr">
@@ -2965,7 +2965,7 @@
       <c r="A70" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="2" t="n">
+      <c r="B70" s="4" t="n">
         <v>45867</v>
       </c>
       <c r="C70" t="inlineStr">
@@ -3001,7 +3001,7 @@
       <c r="A71" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="2" t="n">
+      <c r="B71" s="4" t="n">
         <v>45827</v>
       </c>
       <c r="C71" t="inlineStr">
@@ -3037,7 +3037,7 @@
       <c r="A72" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="2" t="n">
+      <c r="B72" s="4" t="n">
         <v>45832</v>
       </c>
       <c r="C72" t="inlineStr">
@@ -3073,7 +3073,7 @@
       <c r="A73" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="2" t="n">
+      <c r="B73" s="4" t="n">
         <v>45839</v>
       </c>
       <c r="C73" t="inlineStr">
@@ -3109,7 +3109,7 @@
       <c r="A74" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="2" t="n">
+      <c r="B74" s="4" t="n">
         <v>45839</v>
       </c>
       <c r="C74" t="inlineStr">
@@ -3145,7 +3145,7 @@
       <c r="A75" t="n">
         <v>74</v>
       </c>
-      <c r="B75" s="2" t="n">
+      <c r="B75" s="4" t="n">
         <v>45848</v>
       </c>
       <c r="C75" t="inlineStr">
@@ -3181,7 +3181,7 @@
       <c r="A76" t="n">
         <v>75</v>
       </c>
-      <c r="B76" s="2" t="n">
+      <c r="B76" s="4" t="n">
         <v>45849</v>
       </c>
       <c r="C76" t="inlineStr">
@@ -3217,7 +3217,7 @@
       <c r="A77" t="n">
         <v>76</v>
       </c>
-      <c r="B77" s="2" t="n">
+      <c r="B77" s="4" t="n">
         <v>45860</v>
       </c>
       <c r="C77" t="inlineStr">
@@ -3253,7 +3253,7 @@
       <c r="A78" t="n">
         <v>77</v>
       </c>
-      <c r="B78" s="2" t="n">
+      <c r="B78" s="4" t="n">
         <v>45867</v>
       </c>
       <c r="C78" t="inlineStr">
@@ -3289,7 +3289,7 @@
       <c r="A79" t="n">
         <v>78</v>
       </c>
-      <c r="B79" s="2" t="n">
+      <c r="B79" s="4" t="n">
         <v>45867</v>
       </c>
       <c r="C79" t="inlineStr">
@@ -3325,7 +3325,7 @@
       <c r="A80" t="n">
         <v>79</v>
       </c>
-      <c r="B80" s="2" t="n">
+      <c r="B80" s="4" t="n">
         <v>45867</v>
       </c>
       <c r="C80" t="inlineStr">
@@ -3361,7 +3361,7 @@
       <c r="A81" t="n">
         <v>80</v>
       </c>
-      <c r="B81" s="2" t="n">
+      <c r="B81" s="4" t="n">
         <v>45868</v>
       </c>
       <c r="C81" t="inlineStr">
@@ -3397,7 +3397,7 @@
       <c r="A82" t="n">
         <v>81</v>
       </c>
-      <c r="B82" s="2" t="n">
+      <c r="B82" s="4" t="n">
         <v>45870</v>
       </c>
       <c r="C82" t="inlineStr">
@@ -3433,7 +3433,7 @@
       <c r="A83" t="n">
         <v>82</v>
       </c>
-      <c r="B83" s="2" t="n">
+      <c r="B83" s="4" t="n">
         <v>45877</v>
       </c>
       <c r="C83" t="inlineStr">
@@ -3469,7 +3469,7 @@
       <c r="A84" t="n">
         <v>83</v>
       </c>
-      <c r="B84" s="2" t="n">
+      <c r="B84" s="4" t="n">
         <v>45828</v>
       </c>
       <c r="C84" t="inlineStr">
@@ -3505,7 +3505,7 @@
       <c r="A85" t="n">
         <v>84</v>
       </c>
-      <c r="B85" s="2" t="n">
+      <c r="B85" s="4" t="n">
         <v>45832</v>
       </c>
       <c r="C85" t="inlineStr">
@@ -3541,7 +3541,7 @@
       <c r="A86" t="n">
         <v>85</v>
       </c>
-      <c r="B86" s="2" t="n">
+      <c r="B86" s="4" t="n">
         <v>45834</v>
       </c>
       <c r="C86" t="inlineStr">
@@ -3577,7 +3577,7 @@
       <c r="A87" t="n">
         <v>86</v>
       </c>
-      <c r="B87" s="2" t="n">
+      <c r="B87" s="4" t="n">
         <v>45834</v>
       </c>
       <c r="C87" t="inlineStr">
@@ -3613,7 +3613,7 @@
       <c r="A88" t="n">
         <v>87</v>
       </c>
-      <c r="B88" s="2" t="n">
+      <c r="B88" s="4" t="n">
         <v>45834</v>
       </c>
       <c r="C88" t="inlineStr">
@@ -3649,7 +3649,7 @@
       <c r="A89" t="n">
         <v>88</v>
       </c>
-      <c r="B89" s="2" t="n">
+      <c r="B89" s="4" t="n">
         <v>45835</v>
       </c>
       <c r="C89" t="inlineStr">
@@ -3685,7 +3685,7 @@
       <c r="A90" t="n">
         <v>89</v>
       </c>
-      <c r="B90" s="2" t="n">
+      <c r="B90" s="4" t="n">
         <v>45835</v>
       </c>
       <c r="C90" t="inlineStr">
@@ -3721,7 +3721,7 @@
       <c r="A91" t="n">
         <v>90</v>
       </c>
-      <c r="B91" s="2" t="n">
+      <c r="B91" s="4" t="n">
         <v>45841</v>
       </c>
       <c r="C91" t="inlineStr">
@@ -3757,7 +3757,7 @@
       <c r="A92" t="n">
         <v>91</v>
       </c>
-      <c r="B92" s="2" t="n">
+      <c r="B92" s="4" t="n">
         <v>45841</v>
       </c>
       <c r="C92" t="inlineStr">
@@ -3793,7 +3793,7 @@
       <c r="A93" t="n">
         <v>92</v>
       </c>
-      <c r="B93" s="2" t="n">
+      <c r="B93" s="4" t="n">
         <v>45843</v>
       </c>
       <c r="C93" t="inlineStr">
@@ -3829,7 +3829,7 @@
       <c r="A94" t="n">
         <v>93</v>
       </c>
-      <c r="B94" s="2" t="n">
+      <c r="B94" s="4" t="n">
         <v>45848</v>
       </c>
       <c r="C94" t="inlineStr">
@@ -3865,7 +3865,7 @@
       <c r="A95" t="n">
         <v>94</v>
       </c>
-      <c r="B95" s="2" t="n">
+      <c r="B95" s="4" t="n">
         <v>45848</v>
       </c>
       <c r="C95" t="inlineStr">
@@ -3901,7 +3901,7 @@
       <c r="A96" t="n">
         <v>95</v>
       </c>
-      <c r="B96" s="2" t="n">
+      <c r="B96" s="4" t="n">
         <v>45861</v>
       </c>
       <c r="C96" t="inlineStr">
@@ -3937,7 +3937,7 @@
       <c r="A97" t="n">
         <v>96</v>
       </c>
-      <c r="B97" s="2" t="n">
+      <c r="B97" s="4" t="n">
         <v>45863</v>
       </c>
       <c r="C97" t="inlineStr">
@@ -3973,7 +3973,7 @@
       <c r="A98" t="n">
         <v>97</v>
       </c>
-      <c r="B98" s="2" t="n">
+      <c r="B98" s="4" t="n">
         <v>45815</v>
       </c>
       <c r="C98" t="inlineStr">
@@ -4009,7 +4009,7 @@
       <c r="A99" t="n">
         <v>98</v>
       </c>
-      <c r="B99" s="2" t="n">
+      <c r="B99" s="4" t="n">
         <v>45813</v>
       </c>
       <c r="C99" t="inlineStr">
@@ -4045,7 +4045,7 @@
       <c r="A100" t="n">
         <v>99</v>
       </c>
-      <c r="B100" s="2" t="n">
+      <c r="B100" s="4" t="n">
         <v>45814</v>
       </c>
       <c r="C100" t="inlineStr">
@@ -4081,7 +4081,7 @@
       <c r="A101" t="n">
         <v>100</v>
       </c>
-      <c r="B101" s="2" t="n">
+      <c r="B101" s="4" t="n">
         <v>45814</v>
       </c>
       <c r="C101" t="inlineStr">
@@ -4117,7 +4117,7 @@
       <c r="A102" t="n">
         <v>101</v>
       </c>
-      <c r="B102" s="2" t="n">
+      <c r="B102" s="4" t="n">
         <v>45815</v>
       </c>
       <c r="C102" t="inlineStr">
@@ -4153,7 +4153,7 @@
       <c r="A103" t="n">
         <v>102</v>
       </c>
-      <c r="B103" s="2" t="n">
+      <c r="B103" s="4" t="n">
         <v>45816</v>
       </c>
       <c r="C103" t="inlineStr">
@@ -4189,7 +4189,7 @@
       <c r="A104" t="n">
         <v>103</v>
       </c>
-      <c r="B104" s="2" t="n">
+      <c r="B104" s="4" t="n">
         <v>45816</v>
       </c>
       <c r="C104" t="inlineStr">
@@ -4225,7 +4225,7 @@
       <c r="A105" t="n">
         <v>104</v>
       </c>
-      <c r="B105" s="2" t="n">
+      <c r="B105" s="4" t="n">
         <v>45816</v>
       </c>
       <c r="C105" t="inlineStr">
@@ -4261,7 +4261,7 @@
       <c r="A106" t="n">
         <v>105</v>
       </c>
-      <c r="B106" s="2" t="n">
+      <c r="B106" s="4" t="n">
         <v>45816</v>
       </c>
       <c r="C106" t="inlineStr">
@@ -4297,7 +4297,7 @@
       <c r="A107" t="n">
         <v>106</v>
       </c>
-      <c r="B107" s="2" t="n">
+      <c r="B107" s="4" t="n">
         <v>45819</v>
       </c>
       <c r="C107" t="inlineStr">
@@ -4333,7 +4333,7 @@
       <c r="A108" t="n">
         <v>107</v>
       </c>
-      <c r="B108" s="2" t="n">
+      <c r="B108" s="4" t="n">
         <v>45821</v>
       </c>
       <c r="C108" t="inlineStr">
@@ -4369,7 +4369,7 @@
       <c r="A109" t="n">
         <v>108</v>
       </c>
-      <c r="B109" s="2" t="n">
+      <c r="B109" s="4" t="n">
         <v>45822</v>
       </c>
       <c r="C109" t="inlineStr">
@@ -4405,7 +4405,7 @@
       <c r="A110" t="n">
         <v>109</v>
       </c>
-      <c r="B110" s="2" t="n">
+      <c r="B110" s="4" t="n">
         <v>45822</v>
       </c>
       <c r="C110" t="inlineStr">
@@ -4441,7 +4441,7 @@
       <c r="A111" t="n">
         <v>110</v>
       </c>
-      <c r="B111" s="2" t="n">
+      <c r="B111" s="4" t="n">
         <v>45826</v>
       </c>
       <c r="C111" t="inlineStr">
@@ -4477,7 +4477,7 @@
       <c r="A112" t="n">
         <v>111</v>
       </c>
-      <c r="B112" s="2" t="n">
+      <c r="B112" s="4" t="n">
         <v>45835</v>
       </c>
       <c r="C112" t="inlineStr">
@@ -4513,7 +4513,7 @@
       <c r="A113" t="n">
         <v>112</v>
       </c>
-      <c r="B113" s="2" t="n">
+      <c r="B113" s="4" t="n">
         <v>45835</v>
       </c>
       <c r="C113" t="inlineStr">
@@ -4549,7 +4549,7 @@
       <c r="A114" t="n">
         <v>113</v>
       </c>
-      <c r="B114" s="2" t="n">
+      <c r="B114" s="4" t="n">
         <v>45848</v>
       </c>
       <c r="C114" t="inlineStr">
@@ -4585,7 +4585,7 @@
       <c r="A115" t="n">
         <v>114</v>
       </c>
-      <c r="B115" s="2" t="n">
+      <c r="B115" s="4" t="n">
         <v>45842</v>
       </c>
       <c r="C115" t="inlineStr">
@@ -4621,7 +4621,7 @@
       <c r="A116" t="n">
         <v>115</v>
       </c>
-      <c r="B116" s="2" t="n">
+      <c r="B116" s="4" t="n">
         <v>45842</v>
       </c>
       <c r="C116" t="inlineStr">
@@ -4657,7 +4657,7 @@
       <c r="A117" t="n">
         <v>116</v>
       </c>
-      <c r="B117" s="2" t="n">
+      <c r="B117" s="4" t="n">
         <v>45842</v>
       </c>
       <c r="C117" t="inlineStr">
@@ -4693,7 +4693,7 @@
       <c r="A118" t="n">
         <v>117</v>
       </c>
-      <c r="B118" s="2" t="n">
+      <c r="B118" s="4" t="n">
         <v>45843</v>
       </c>
       <c r="C118" t="inlineStr">
@@ -4729,7 +4729,7 @@
       <c r="A119" t="n">
         <v>118</v>
       </c>
-      <c r="B119" s="2" t="n">
+      <c r="B119" s="4" t="n">
         <v>45843</v>
       </c>
       <c r="C119" t="inlineStr">
@@ -4765,7 +4765,7 @@
       <c r="A120" t="n">
         <v>119</v>
       </c>
-      <c r="B120" s="2" t="n">
+      <c r="B120" s="4" t="n">
         <v>45846</v>
       </c>
       <c r="C120" t="inlineStr">
@@ -4801,7 +4801,7 @@
       <c r="A121" t="n">
         <v>120</v>
       </c>
-      <c r="B121" s="2" t="n">
+      <c r="B121" s="4" t="n">
         <v>45847</v>
       </c>
       <c r="C121" t="inlineStr">
@@ -4837,7 +4837,7 @@
       <c r="A122" t="n">
         <v>121</v>
       </c>
-      <c r="B122" s="2" t="n">
+      <c r="B122" s="4" t="n">
         <v>45849</v>
       </c>
       <c r="C122" t="inlineStr">
@@ -4873,7 +4873,7 @@
       <c r="A123" t="n">
         <v>122</v>
       </c>
-      <c r="B123" s="2" t="n">
+      <c r="B123" s="4" t="n">
         <v>45849</v>
       </c>
       <c r="C123" t="inlineStr">
@@ -4909,7 +4909,7 @@
       <c r="A124" t="n">
         <v>123</v>
       </c>
-      <c r="B124" s="2" t="n">
+      <c r="B124" s="4" t="n">
         <v>45850</v>
       </c>
       <c r="C124" t="inlineStr">
@@ -4945,7 +4945,7 @@
       <c r="A125" t="n">
         <v>124</v>
       </c>
-      <c r="B125" s="2" t="n">
+      <c r="B125" s="4" t="n">
         <v>45863</v>
       </c>
       <c r="C125" t="inlineStr">
@@ -4981,7 +4981,7 @@
       <c r="A126" t="n">
         <v>125</v>
       </c>
-      <c r="B126" s="2" t="n">
+      <c r="B126" s="4" t="n">
         <v>45867</v>
       </c>
       <c r="C126" t="inlineStr">
@@ -5017,7 +5017,7 @@
       <c r="A127" t="n">
         <v>126</v>
       </c>
-      <c r="B127" s="2" t="n">
+      <c r="B127" s="4" t="n">
         <v>45863</v>
       </c>
       <c r="C127" t="inlineStr">
@@ -5053,7 +5053,7 @@
       <c r="A128" t="n">
         <v>127</v>
       </c>
-      <c r="B128" s="2" t="n">
+      <c r="B128" s="4" t="n">
         <v>45867</v>
       </c>
       <c r="C128" t="inlineStr">
@@ -5089,7 +5089,7 @@
       <c r="A129" t="n">
         <v>128</v>
       </c>
-      <c r="B129" s="2" t="n">
+      <c r="B129" s="4" t="n">
         <v>45869</v>
       </c>
       <c r="C129" t="inlineStr">
@@ -5125,7 +5125,7 @@
       <c r="A130" t="n">
         <v>129</v>
       </c>
-      <c r="B130" s="2" t="n">
+      <c r="B130" s="4" t="n">
         <v>45870</v>
       </c>
       <c r="C130" t="inlineStr">
@@ -5161,7 +5161,7 @@
       <c r="A131" t="n">
         <v>130</v>
       </c>
-      <c r="B131" s="2" t="n">
+      <c r="B131" s="4" t="n">
         <v>45875</v>
       </c>
       <c r="C131" t="inlineStr">
@@ -5197,7 +5197,7 @@
       <c r="A132" t="n">
         <v>131</v>
       </c>
-      <c r="B132" s="2" t="n">
+      <c r="B132" s="4" t="n">
         <v>45869</v>
       </c>
       <c r="C132" t="inlineStr">
@@ -5233,7 +5233,7 @@
       <c r="A133" t="n">
         <v>132</v>
       </c>
-      <c r="B133" s="2" t="n">
+      <c r="B133" s="4" t="n">
         <v>45869</v>
       </c>
       <c r="C133" t="inlineStr">
@@ -5269,7 +5269,7 @@
       <c r="A134" t="n">
         <v>133</v>
       </c>
-      <c r="B134" s="2" t="n">
+      <c r="B134" s="4" t="n">
         <v>45869</v>
       </c>
       <c r="C134" t="inlineStr">
@@ -5305,7 +5305,7 @@
       <c r="A135" t="n">
         <v>134</v>
       </c>
-      <c r="B135" s="2" t="n">
+      <c r="B135" s="4" t="n">
         <v>45869</v>
       </c>
       <c r="C135" t="inlineStr">
@@ -5341,7 +5341,7 @@
       <c r="A136" t="n">
         <v>135</v>
       </c>
-      <c r="B136" s="2" t="n">
+      <c r="B136" s="4" t="n">
         <v>45869</v>
       </c>
       <c r="C136" t="inlineStr">
@@ -5377,7 +5377,7 @@
       <c r="A137" t="n">
         <v>136</v>
       </c>
-      <c r="B137" s="2" t="n">
+      <c r="B137" s="4" t="n">
         <v>45870</v>
       </c>
       <c r="C137" t="inlineStr">
@@ -5413,7 +5413,7 @@
       <c r="A138" t="n">
         <v>137</v>
       </c>
-      <c r="B138" s="2" t="n">
+      <c r="B138" s="4" t="n">
         <v>45870</v>
       </c>
       <c r="C138" t="inlineStr">
@@ -5449,7 +5449,7 @@
       <c r="A139" t="n">
         <v>138</v>
       </c>
-      <c r="B139" s="2" t="n">
+      <c r="B139" s="4" t="n">
         <v>45872</v>
       </c>
       <c r="C139" t="inlineStr">
@@ -5485,7 +5485,7 @@
       <c r="A140" t="n">
         <v>139</v>
       </c>
-      <c r="B140" s="2" t="n">
+      <c r="B140" s="4" t="n">
         <v>45873</v>
       </c>
       <c r="C140" t="inlineStr">
@@ -5521,7 +5521,7 @@
       <c r="A141" t="n">
         <v>140</v>
       </c>
-      <c r="B141" s="2" t="n">
+      <c r="B141" s="4" t="n">
         <v>45873</v>
       </c>
       <c r="C141" t="inlineStr">
@@ -5557,7 +5557,7 @@
       <c r="A142" t="n">
         <v>141</v>
       </c>
-      <c r="B142" s="2" t="n">
+      <c r="B142" s="4" t="n">
         <v>45877</v>
       </c>
       <c r="C142" t="inlineStr">
@@ -5593,7 +5593,7 @@
       <c r="A143" t="n">
         <v>142</v>
       </c>
-      <c r="B143" s="2" t="n">
+      <c r="B143" s="4" t="n">
         <v>45875</v>
       </c>
       <c r="C143" t="inlineStr">
@@ -5629,7 +5629,7 @@
       <c r="A144" t="n">
         <v>143</v>
       </c>
-      <c r="B144" s="2" t="n">
+      <c r="B144" s="4" t="n">
         <v>45875</v>
       </c>
       <c r="C144" t="inlineStr">
@@ -5665,7 +5665,7 @@
       <c r="A145" t="n">
         <v>144</v>
       </c>
-      <c r="B145" s="2" t="n">
+      <c r="B145" s="4" t="n">
         <v>45875</v>
       </c>
       <c r="C145" t="inlineStr">
@@ -5701,7 +5701,7 @@
       <c r="A146" t="n">
         <v>145</v>
       </c>
-      <c r="B146" s="2" t="n">
+      <c r="B146" s="4" t="n">
         <v>45875</v>
       </c>
       <c r="C146" t="inlineStr">
@@ -5737,7 +5737,7 @@
       <c r="A147" t="n">
         <v>146</v>
       </c>
-      <c r="B147" s="2" t="n">
+      <c r="B147" s="4" t="n">
         <v>45877</v>
       </c>
       <c r="C147" t="inlineStr">
@@ -5773,7 +5773,7 @@
       <c r="A148" t="n">
         <v>147</v>
       </c>
-      <c r="B148" s="2" t="n">
+      <c r="B148" s="4" t="n">
         <v>45860</v>
       </c>
       <c r="C148" t="inlineStr">
@@ -5809,7 +5809,7 @@
       <c r="A149" t="n">
         <v>148</v>
       </c>
-      <c r="B149" s="2" t="n">
+      <c r="B149" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C149" t="inlineStr">
@@ -5845,7 +5845,7 @@
       <c r="A150" t="n">
         <v>149</v>
       </c>
-      <c r="B150" s="2" t="n">
+      <c r="B150" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C150" t="inlineStr">
@@ -5881,7 +5881,7 @@
       <c r="A151" t="n">
         <v>150</v>
       </c>
-      <c r="B151" s="2" t="n">
+      <c r="B151" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C151" t="inlineStr">
@@ -5917,7 +5917,7 @@
       <c r="A152" t="n">
         <v>151</v>
       </c>
-      <c r="B152" s="2" t="n">
+      <c r="B152" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C152" t="inlineStr">
@@ -5953,7 +5953,7 @@
       <c r="A153" t="n">
         <v>152</v>
       </c>
-      <c r="B153" s="2" t="n">
+      <c r="B153" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C153" t="inlineStr">
@@ -5989,7 +5989,7 @@
       <c r="A154" t="n">
         <v>153</v>
       </c>
-      <c r="B154" s="2" t="n">
+      <c r="B154" s="4" t="n">
         <v>45890</v>
       </c>
       <c r="C154" t="inlineStr">
@@ -6025,7 +6025,7 @@
       <c r="A155" t="n">
         <v>154</v>
       </c>
-      <c r="B155" s="2" t="n">
+      <c r="B155" s="4" t="n">
         <v>45890</v>
       </c>
       <c r="C155" t="inlineStr">
@@ -6061,7 +6061,7 @@
       <c r="A156" t="n">
         <v>155</v>
       </c>
-      <c r="B156" s="2" t="n">
+      <c r="B156" s="4" t="n">
         <v>45897</v>
       </c>
       <c r="C156" t="inlineStr">
@@ -6097,7 +6097,7 @@
       <c r="A157" t="n">
         <v>156</v>
       </c>
-      <c r="B157" s="2" t="n">
+      <c r="B157" s="4" t="n">
         <v>45897</v>
       </c>
       <c r="C157" t="inlineStr">
@@ -6133,7 +6133,7 @@
       <c r="A158" t="n">
         <v>157</v>
       </c>
-      <c r="B158" s="2" t="n">
+      <c r="B158" s="4" t="n">
         <v>45897</v>
       </c>
       <c r="C158" t="inlineStr">
@@ -6169,7 +6169,7 @@
       <c r="A159" t="n">
         <v>158</v>
       </c>
-      <c r="B159" s="2" t="n">
+      <c r="B159" s="4" t="n">
         <v>45875</v>
       </c>
       <c r="C159" t="inlineStr">
@@ -6205,7 +6205,7 @@
       <c r="A160" t="n">
         <v>159</v>
       </c>
-      <c r="B160" s="2" t="n">
+      <c r="B160" s="4" t="n">
         <v>45875</v>
       </c>
       <c r="C160" t="inlineStr">
@@ -6241,7 +6241,7 @@
       <c r="A161" t="n">
         <v>160</v>
       </c>
-      <c r="B161" s="2" t="n">
+      <c r="B161" s="4" t="n">
         <v>45914</v>
       </c>
       <c r="C161" t="inlineStr">
@@ -6277,7 +6277,7 @@
       <c r="A162" t="n">
         <v>161</v>
       </c>
-      <c r="B162" s="2" t="n">
+      <c r="B162" s="4" t="n">
         <v>45890</v>
       </c>
       <c r="C162" t="inlineStr">
@@ -6313,7 +6313,7 @@
       <c r="A163" t="n">
         <v>162</v>
       </c>
-      <c r="B163" s="2" t="n">
+      <c r="B163" s="4" t="n">
         <v>45890</v>
       </c>
       <c r="C163" t="inlineStr">
@@ -6349,7 +6349,7 @@
       <c r="A164" t="n">
         <v>163</v>
       </c>
-      <c r="B164" s="2" t="n">
+      <c r="B164" s="4" t="n">
         <v>45896</v>
       </c>
       <c r="C164" t="inlineStr">
@@ -6385,7 +6385,7 @@
       <c r="A165" t="n">
         <v>164</v>
       </c>
-      <c r="B165" s="2" t="n">
+      <c r="B165" s="4" t="n">
         <v>45904</v>
       </c>
       <c r="C165" t="inlineStr">
@@ -6421,7 +6421,7 @@
       <c r="A166" t="n">
         <v>165</v>
       </c>
-      <c r="B166" s="2" t="n">
+      <c r="B166" s="4" t="n">
         <v>45879</v>
       </c>
       <c r="C166" t="inlineStr">
@@ -6457,7 +6457,7 @@
       <c r="A167" t="n">
         <v>166</v>
       </c>
-      <c r="B167" s="2" t="n">
+      <c r="B167" s="4" t="n">
         <v>45875</v>
       </c>
       <c r="C167" t="inlineStr">
@@ -6493,7 +6493,7 @@
       <c r="A168" t="n">
         <v>167</v>
       </c>
-      <c r="B168" s="2" t="n">
+      <c r="B168" s="4" t="n">
         <v>45881</v>
       </c>
       <c r="C168" t="inlineStr">
@@ -6529,7 +6529,7 @@
       <c r="A169" t="n">
         <v>168</v>
       </c>
-      <c r="B169" s="2" t="n">
+      <c r="B169" s="4" t="n">
         <v>45888</v>
       </c>
       <c r="C169" t="inlineStr">
@@ -6565,7 +6565,7 @@
       <c r="A170" t="n">
         <v>169</v>
       </c>
-      <c r="B170" s="2" t="n">
+      <c r="B170" s="4" t="n">
         <v>45889</v>
       </c>
       <c r="C170" t="inlineStr">
@@ -6601,7 +6601,7 @@
       <c r="A171" t="n">
         <v>170</v>
       </c>
-      <c r="B171" s="2" t="n">
+      <c r="B171" s="4" t="n">
         <v>45890</v>
       </c>
       <c r="C171" t="inlineStr">
@@ -6637,7 +6637,7 @@
       <c r="A172" t="n">
         <v>171</v>
       </c>
-      <c r="B172" s="2" t="n">
+      <c r="B172" s="4" t="n">
         <v>45895</v>
       </c>
       <c r="C172" t="inlineStr">
@@ -6673,7 +6673,7 @@
       <c r="A173" t="n">
         <v>172</v>
       </c>
-      <c r="B173" s="2" t="n">
+      <c r="B173" s="4" t="n">
         <v>45895</v>
       </c>
       <c r="C173" t="inlineStr">
@@ -6709,7 +6709,7 @@
       <c r="A174" t="n">
         <v>173</v>
       </c>
-      <c r="B174" s="2" t="n">
+      <c r="B174" s="4" t="n">
         <v>45877</v>
       </c>
       <c r="C174" t="inlineStr">
@@ -6745,7 +6745,7 @@
       <c r="A175" t="n">
         <v>174</v>
       </c>
-      <c r="B175" s="2" t="n">
+      <c r="B175" s="4" t="n">
         <v>45877</v>
       </c>
       <c r="C175" t="inlineStr">
@@ -6781,7 +6781,7 @@
       <c r="A176" t="n">
         <v>175</v>
       </c>
-      <c r="B176" s="2" t="n">
+      <c r="B176" s="4" t="n">
         <v>45877</v>
       </c>
       <c r="C176" t="inlineStr">
@@ -6817,7 +6817,7 @@
       <c r="A177" t="n">
         <v>176</v>
       </c>
-      <c r="B177" s="2" t="n">
+      <c r="B177" s="4" t="n">
         <v>45877</v>
       </c>
       <c r="C177" t="inlineStr">
@@ -6853,7 +6853,7 @@
       <c r="A178" t="n">
         <v>177</v>
       </c>
-      <c r="B178" s="2" t="n">
+      <c r="B178" s="4" t="n">
         <v>45877</v>
       </c>
       <c r="C178" t="inlineStr">
@@ -6889,7 +6889,7 @@
       <c r="A179" t="n">
         <v>178</v>
       </c>
-      <c r="B179" s="2" t="n">
+      <c r="B179" s="4" t="n">
         <v>45881</v>
       </c>
       <c r="C179" t="inlineStr">
@@ -6925,7 +6925,7 @@
       <c r="A180" t="n">
         <v>179</v>
       </c>
-      <c r="B180" s="2" t="n">
+      <c r="B180" s="4" t="n">
         <v>45885</v>
       </c>
       <c r="C180" t="inlineStr">
@@ -6961,7 +6961,7 @@
       <c r="A181" t="n">
         <v>180</v>
       </c>
-      <c r="B181" s="2" t="n">
+      <c r="B181" s="4" t="n">
         <v>45856</v>
       </c>
       <c r="C181" t="inlineStr">
@@ -6997,7 +6997,7 @@
       <c r="A182" t="n">
         <v>181</v>
       </c>
-      <c r="B182" s="2" t="n">
+      <c r="B182" s="4" t="n">
         <v>45879</v>
       </c>
       <c r="C182" t="inlineStr">
@@ -7033,7 +7033,7 @@
       <c r="A183" t="n">
         <v>182</v>
       </c>
-      <c r="B183" s="2" t="n">
+      <c r="B183" s="4" t="n">
         <v>45886</v>
       </c>
       <c r="C183" t="inlineStr">
@@ -7069,7 +7069,7 @@
       <c r="A184" t="n">
         <v>183</v>
       </c>
-      <c r="B184" s="2" t="n">
+      <c r="B184" s="4" t="n">
         <v>45885</v>
       </c>
       <c r="C184" t="inlineStr">
@@ -7105,7 +7105,7 @@
       <c r="A185" t="n">
         <v>184</v>
       </c>
-      <c r="B185" s="2" t="n">
+      <c r="B185" s="4" t="n">
         <v>45901</v>
       </c>
       <c r="C185" t="inlineStr">
@@ -7141,7 +7141,7 @@
       <c r="A186" t="n">
         <v>185</v>
       </c>
-      <c r="B186" s="2" t="n">
+      <c r="B186" s="4" t="n">
         <v>45855</v>
       </c>
       <c r="C186" t="inlineStr">
@@ -7177,7 +7177,7 @@
       <c r="A187" t="n">
         <v>186</v>
       </c>
-      <c r="B187" s="2" t="n">
+      <c r="B187" s="4" t="n">
         <v>45885</v>
       </c>
       <c r="C187" t="inlineStr">
@@ -7213,7 +7213,7 @@
       <c r="A188" t="n">
         <v>187</v>
       </c>
-      <c r="B188" s="2" t="n">
+      <c r="B188" s="4" t="n">
         <v>45888</v>
       </c>
       <c r="C188" t="inlineStr">
@@ -7249,7 +7249,7 @@
       <c r="A189" t="n">
         <v>188</v>
       </c>
-      <c r="B189" s="2" t="n">
+      <c r="B189" s="4" t="n">
         <v>45889</v>
       </c>
       <c r="C189" t="inlineStr">
@@ -7285,7 +7285,7 @@
       <c r="A190" t="n">
         <v>189</v>
       </c>
-      <c r="B190" s="2" t="n">
+      <c r="B190" s="4" t="n">
         <v>45892</v>
       </c>
       <c r="C190" t="inlineStr">
@@ -7321,7 +7321,7 @@
       <c r="A191" t="n">
         <v>190</v>
       </c>
-      <c r="B191" s="2" t="n">
+      <c r="B191" s="4" t="n">
         <v>45855</v>
       </c>
       <c r="C191" t="inlineStr">
@@ -7357,7 +7357,7 @@
       <c r="A192" t="n">
         <v>191</v>
       </c>
-      <c r="B192" s="2" t="n">
+      <c r="B192" s="4" t="n">
         <v>45855</v>
       </c>
       <c r="C192" t="inlineStr">
@@ -7393,7 +7393,7 @@
       <c r="A193" t="n">
         <v>192</v>
       </c>
-      <c r="B193" s="2" t="n">
+      <c r="B193" s="4" t="n">
         <v>45855</v>
       </c>
       <c r="C193" t="inlineStr">
@@ -7429,7 +7429,7 @@
       <c r="A194" t="n">
         <v>193</v>
       </c>
-      <c r="B194" s="2" t="n">
+      <c r="B194" s="4" t="n">
         <v>45896</v>
       </c>
       <c r="C194" t="inlineStr">
@@ -7465,7 +7465,7 @@
       <c r="A195" t="n">
         <v>194</v>
       </c>
-      <c r="B195" s="2" t="n">
+      <c r="B195" s="4" t="n">
         <v>45901</v>
       </c>
       <c r="C195" t="inlineStr">
@@ -7501,7 +7501,7 @@
       <c r="A196" t="n">
         <v>195</v>
       </c>
-      <c r="B196" s="2" t="n">
+      <c r="B196" s="4" t="n">
         <v>45905</v>
       </c>
       <c r="C196" t="inlineStr">
@@ -7537,7 +7537,7 @@
       <c r="A197" t="n">
         <v>196</v>
       </c>
-      <c r="B197" s="2" t="n">
+      <c r="B197" s="4" t="n">
         <v>45905</v>
       </c>
       <c r="C197" t="inlineStr">
@@ -7573,7 +7573,7 @@
       <c r="A198" t="n">
         <v>197</v>
       </c>
-      <c r="B198" s="2" t="n">
+      <c r="B198" s="4" t="n">
         <v>45905</v>
       </c>
       <c r="C198" t="inlineStr">
@@ -7609,7 +7609,7 @@
       <c r="A199" t="n">
         <v>198</v>
       </c>
-      <c r="B199" s="2" t="n">
+      <c r="B199" s="4" t="n">
         <v>45905</v>
       </c>
       <c r="C199" t="inlineStr">
@@ -7645,7 +7645,7 @@
       <c r="A200" t="n">
         <v>199</v>
       </c>
-      <c r="B200" s="2" t="n">
+      <c r="B200" s="4" t="n">
         <v>45905</v>
       </c>
       <c r="C200" t="inlineStr">
@@ -7681,7 +7681,7 @@
       <c r="A201" t="n">
         <v>200</v>
       </c>
-      <c r="B201" s="2" t="n">
+      <c r="B201" s="4" t="n">
         <v>45905</v>
       </c>
       <c r="C201" t="inlineStr">
@@ -7717,7 +7717,7 @@
       <c r="A202" t="n">
         <v>201</v>
       </c>
-      <c r="B202" s="2" t="n">
+      <c r="B202" s="4" t="n">
         <v>45905</v>
       </c>
       <c r="C202" t="inlineStr">
@@ -7753,7 +7753,7 @@
       <c r="A203" t="n">
         <v>202</v>
       </c>
-      <c r="B203" s="2" t="n">
+      <c r="B203" s="4" t="n">
         <v>45906</v>
       </c>
       <c r="C203" t="inlineStr">
@@ -7789,7 +7789,7 @@
       <c r="A204" t="n">
         <v>203</v>
       </c>
-      <c r="B204" s="2" t="n">
+      <c r="B204" s="4" t="n">
         <v>45909</v>
       </c>
       <c r="C204" t="inlineStr">
@@ -7825,7 +7825,7 @@
       <c r="A205" t="n">
         <v>204</v>
       </c>
-      <c r="B205" s="2" t="n">
+      <c r="B205" s="4" t="n">
         <v>45910</v>
       </c>
       <c r="C205" t="inlineStr">
@@ -7861,7 +7861,7 @@
       <c r="A206" t="n">
         <v>205</v>
       </c>
-      <c r="B206" s="2" t="n">
+      <c r="B206" s="4" t="n">
         <v>45909</v>
       </c>
       <c r="C206" t="inlineStr">
@@ -7897,7 +7897,7 @@
       <c r="A207" t="n">
         <v>206</v>
       </c>
-      <c r="B207" s="2" t="n">
+      <c r="B207" s="4" t="n">
         <v>45909</v>
       </c>
       <c r="C207" t="inlineStr">
@@ -7933,7 +7933,7 @@
       <c r="A208" t="n">
         <v>207</v>
       </c>
-      <c r="B208" s="2" t="n">
+      <c r="B208" s="4" t="n">
         <v>45910</v>
       </c>
       <c r="C208" t="inlineStr">
@@ -7969,7 +7969,7 @@
       <c r="A209" t="n">
         <v>208</v>
       </c>
-      <c r="B209" s="2" t="n">
+      <c r="B209" s="4" t="n">
         <v>45878</v>
       </c>
       <c r="C209" t="inlineStr">
@@ -8005,7 +8005,7 @@
       <c r="A210" t="n">
         <v>209</v>
       </c>
-      <c r="B210" s="2" t="n">
+      <c r="B210" s="4" t="n">
         <v>45878</v>
       </c>
       <c r="C210" t="inlineStr">
@@ -8041,7 +8041,7 @@
       <c r="A211" t="n">
         <v>210</v>
       </c>
-      <c r="B211" s="2" t="n">
+      <c r="B211" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C211" t="inlineStr">
@@ -8077,7 +8077,7 @@
       <c r="A212" t="n">
         <v>211</v>
       </c>
-      <c r="B212" s="2" t="n">
+      <c r="B212" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C212" t="inlineStr">
@@ -8113,7 +8113,7 @@
       <c r="A213" t="n">
         <v>212</v>
       </c>
-      <c r="B213" s="2" t="n">
+      <c r="B213" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C213" t="inlineStr">
@@ -8149,7 +8149,7 @@
       <c r="A214" t="n">
         <v>213</v>
       </c>
-      <c r="B214" s="2" t="n">
+      <c r="B214" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C214" t="inlineStr">
@@ -8185,7 +8185,7 @@
       <c r="A215" t="n">
         <v>214</v>
       </c>
-      <c r="B215" s="2" t="n">
+      <c r="B215" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C215" t="inlineStr">
@@ -8221,7 +8221,7 @@
       <c r="A216" t="n">
         <v>215</v>
       </c>
-      <c r="B216" s="2" t="n">
+      <c r="B216" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C216" t="inlineStr">
@@ -8257,7 +8257,7 @@
       <c r="A217" t="n">
         <v>216</v>
       </c>
-      <c r="B217" s="2" t="n">
+      <c r="B217" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C217" t="inlineStr">
@@ -8293,7 +8293,7 @@
       <c r="A218" t="n">
         <v>217</v>
       </c>
-      <c r="B218" s="2" t="n">
+      <c r="B218" s="4" t="n">
         <v>45910</v>
       </c>
       <c r="C218" t="inlineStr">
@@ -8329,7 +8329,7 @@
       <c r="A219" t="n">
         <v>218</v>
       </c>
-      <c r="B219" s="2" t="n">
+      <c r="B219" s="4" t="n">
         <v>45910</v>
       </c>
       <c r="C219" t="inlineStr">
@@ -8365,7 +8365,7 @@
       <c r="A220" t="n">
         <v>219</v>
       </c>
-      <c r="B220" s="2" t="n">
+      <c r="B220" s="4" t="n">
         <v>45909</v>
       </c>
       <c r="C220" t="inlineStr">
@@ -8401,7 +8401,7 @@
       <c r="A221" t="n">
         <v>220</v>
       </c>
-      <c r="B221" s="2" t="n">
+      <c r="B221" s="4" t="n">
         <v>45909</v>
       </c>
       <c r="C221" t="inlineStr">
@@ -8437,7 +8437,7 @@
       <c r="A222" t="n">
         <v>221</v>
       </c>
-      <c r="B222" s="2" t="n">
+      <c r="B222" s="4" t="n">
         <v>45910</v>
       </c>
       <c r="C222" t="inlineStr">
@@ -8473,7 +8473,7 @@
       <c r="A223" t="n">
         <v>222</v>
       </c>
-      <c r="B223" s="2" t="n">
+      <c r="B223" s="4" t="n">
         <v>45890</v>
       </c>
       <c r="C223" t="inlineStr">
@@ -8509,7 +8509,7 @@
       <c r="A224" t="n">
         <v>223</v>
       </c>
-      <c r="B224" s="2" t="n">
+      <c r="B224" s="4" t="n">
         <v>45890</v>
       </c>
       <c r="C224" t="inlineStr">
@@ -8545,7 +8545,7 @@
       <c r="A225" t="n">
         <v>224</v>
       </c>
-      <c r="B225" s="2" t="n">
+      <c r="B225" s="4" t="n">
         <v>45898</v>
       </c>
       <c r="C225" t="inlineStr">
@@ -8581,7 +8581,7 @@
       <c r="A226" t="n">
         <v>225</v>
       </c>
-      <c r="B226" s="2" t="n">
+      <c r="B226" s="4" t="n">
         <v>45930</v>
       </c>
       <c r="C226" t="inlineStr">
@@ -8617,7 +8617,7 @@
       <c r="A227" t="n">
         <v>226</v>
       </c>
-      <c r="B227" s="2" t="n">
+      <c r="B227" s="4" t="n">
         <v>45911</v>
       </c>
       <c r="C227" t="inlineStr">
@@ -8653,7 +8653,7 @@
       <c r="A228" t="n">
         <v>227</v>
       </c>
-      <c r="B228" s="2" t="n">
+      <c r="B228" s="4" t="n">
         <v>45883</v>
       </c>
       <c r="C228" t="inlineStr">
@@ -8689,7 +8689,7 @@
       <c r="A229" t="n">
         <v>228</v>
       </c>
-      <c r="B229" s="2" t="n">
+      <c r="B229" s="4" t="n">
         <v>45890</v>
       </c>
       <c r="C229" t="inlineStr">
@@ -8725,7 +8725,7 @@
       <c r="A230" t="n">
         <v>229</v>
       </c>
-      <c r="B230" s="2" t="n">
+      <c r="B230" s="4" t="n">
         <v>45879</v>
       </c>
       <c r="C230" t="inlineStr">
@@ -8761,7 +8761,7 @@
       <c r="A231" t="n">
         <v>230</v>
       </c>
-      <c r="B231" s="2" t="n">
+      <c r="B231" s="4" t="n">
         <v>45892</v>
       </c>
       <c r="C231" t="inlineStr">
@@ -8797,7 +8797,7 @@
       <c r="A232" t="n">
         <v>231</v>
       </c>
-      <c r="B232" s="2" t="n">
+      <c r="B232" s="4" t="n">
         <v>45896</v>
       </c>
       <c r="C232" t="inlineStr">
@@ -8833,7 +8833,7 @@
       <c r="A233" t="n">
         <v>232</v>
       </c>
-      <c r="B233" s="2" t="n">
+      <c r="B233" s="4" t="n">
         <v>45893</v>
       </c>
       <c r="C233" t="inlineStr">
@@ -8869,7 +8869,7 @@
       <c r="A234" t="n">
         <v>233</v>
       </c>
-      <c r="B234" s="2" t="n">
+      <c r="B234" s="4" t="n">
         <v>45927</v>
       </c>
       <c r="C234" t="inlineStr">
@@ -8905,7 +8905,7 @@
       <c r="A235" t="n">
         <v>234</v>
       </c>
-      <c r="B235" s="2" t="n">
+      <c r="B235" s="4" t="n">
         <v>45896</v>
       </c>
       <c r="C235" t="inlineStr">
@@ -8941,7 +8941,7 @@
       <c r="A236" t="n">
         <v>235</v>
       </c>
-      <c r="B236" s="2" t="n">
+      <c r="B236" s="4" t="n">
         <v>45912</v>
       </c>
       <c r="C236" t="inlineStr">
@@ -8977,7 +8977,7 @@
       <c r="A237" t="n">
         <v>236</v>
       </c>
-      <c r="B237" s="2" t="n">
+      <c r="B237" s="4" t="n">
         <v>45912</v>
       </c>
       <c r="C237" t="inlineStr">
@@ -9013,7 +9013,7 @@
       <c r="A238" t="n">
         <v>237</v>
       </c>
-      <c r="B238" s="2" t="n">
+      <c r="B238" s="4" t="n">
         <v>45913</v>
       </c>
       <c r="C238" t="inlineStr">
@@ -9049,7 +9049,7 @@
       <c r="A239" t="n">
         <v>238</v>
       </c>
-      <c r="B239" s="2" t="n">
+      <c r="B239" s="4" t="n">
         <v>45914</v>
       </c>
       <c r="C239" t="inlineStr">
@@ -9085,7 +9085,7 @@
       <c r="A240" t="n">
         <v>239</v>
       </c>
-      <c r="B240" s="2" t="n">
+      <c r="B240" s="4" t="n">
         <v>45916</v>
       </c>
       <c r="C240" t="inlineStr">
@@ -9121,7 +9121,7 @@
       <c r="A241" t="n">
         <v>240</v>
       </c>
-      <c r="B241" s="2" t="n">
+      <c r="B241" s="4" t="n">
         <v>45916</v>
       </c>
       <c r="C241" t="inlineStr">
@@ -9157,7 +9157,7 @@
       <c r="A242" t="n">
         <v>241</v>
       </c>
-      <c r="B242" s="2" t="n">
+      <c r="B242" s="4" t="n">
         <v>45921</v>
       </c>
       <c r="C242" t="inlineStr">
@@ -9193,7 +9193,7 @@
       <c r="A243" t="n">
         <v>242</v>
       </c>
-      <c r="B243" s="2" t="n">
+      <c r="B243" s="4" t="n">
         <v>45920</v>
       </c>
       <c r="C243" t="inlineStr">
@@ -9229,7 +9229,7 @@
       <c r="A244" t="n">
         <v>243</v>
       </c>
-      <c r="B244" s="2" t="n">
+      <c r="B244" s="4" t="n">
         <v>45921</v>
       </c>
       <c r="C244" t="inlineStr">
@@ -9265,7 +9265,7 @@
       <c r="A245" t="n">
         <v>244</v>
       </c>
-      <c r="B245" s="3" t="n">
+      <c r="B245" s="4" t="n">
         <v>45922</v>
       </c>
       <c r="C245" t="inlineStr">
@@ -9292,6 +9292,294 @@
         </is>
       </c>
       <c r="H245" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>245</v>
+      </c>
+      <c r="B246" s="4" t="n">
+        <v>45924</v>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="F246" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>246</v>
+      </c>
+      <c r="B247" s="4" t="n">
+        <v>45924</v>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F247" t="n">
+        <v>3000</v>
+      </c>
+      <c r="G247" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>247</v>
+      </c>
+      <c r="B248" s="4" t="n">
+        <v>45924</v>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>Factura - la factura se realizo por : 3000  + saldo anterior 7000 = total 10000</t>
+        </is>
+      </c>
+      <c r="F248" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G248" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>248</v>
+      </c>
+      <c r="B249" s="4" t="n">
+        <v>45924</v>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F249" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>249</v>
+      </c>
+      <c r="B250" s="4" t="n">
+        <v>45924</v>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F250" t="n">
+        <v>3500</v>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>250</v>
+      </c>
+      <c r="B251" s="4" t="n">
+        <v>45924</v>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>Factura - la factura se realizo por : 4000  + saldo anterior 1500 = total 5500</t>
+        </is>
+      </c>
+      <c r="F251" t="n">
+        <v>5500</v>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>F-003</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>251</v>
+      </c>
+      <c r="B252" s="4" t="n">
+        <v>45924</v>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F252" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>F-003</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>252</v>
+      </c>
+      <c r="B253" s="5" t="n">
+        <v>45924</v>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Pepito</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="F253" t="n">
+        <v>50000</v>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -9308,7 +9596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:E1"/>
@@ -9512,6 +9800,44 @@
       </c>
       <c r="E10" t="n">
         <v>20128000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>5500</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2500</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Pepito</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>